<commit_message>
update effort with bash
</commit_message>
<xml_diff>
--- a/data/epu.xlsx
+++ b/data/epu.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="27">
   <si>
     <t>year</t>
   </si>
@@ -114,7 +114,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -122,12 +122,14 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -137,7 +139,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C267"/>
+  <dimension ref="A1:C268"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -155,10 +157,10 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="0">
-        <v>1</v>
-      </c>
-      <c r="C2" s="0">
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
         <v>114.2330322265625</v>
       </c>
     </row>
@@ -166,10 +168,10 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="0">
-        <v>2</v>
-      </c>
-      <c r="C3" s="0">
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
         <v>71.152473449707031</v>
       </c>
     </row>
@@ -177,10 +179,10 @@
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="0">
-        <v>3</v>
-      </c>
-      <c r="C4" s="0">
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
         <v>148.08653259277344</v>
       </c>
     </row>
@@ -188,10 +190,10 @@
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="0">
-        <v>4</v>
-      </c>
-      <c r="C5" s="0">
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
         <v>146.97679138183594</v>
       </c>
     </row>
@@ -199,10 +201,10 @@
       <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="0">
-        <v>5</v>
-      </c>
-      <c r="C6" s="0">
+      <c r="B6" s="1">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
         <v>111.51500701904297</v>
       </c>
     </row>
@@ -210,10 +212,10 @@
       <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="0">
-        <v>6</v>
-      </c>
-      <c r="C7" s="0">
+      <c r="B7" s="1">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
         <v>85.492919921875</v>
       </c>
     </row>
@@ -221,10 +223,10 @@
       <c r="A8" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="0">
-        <v>7</v>
-      </c>
-      <c r="C8" s="0">
+      <c r="B8" s="1">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1">
         <v>180.79301452636719</v>
       </c>
     </row>
@@ -232,10 +234,10 @@
       <c r="A9" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="0">
-        <v>8</v>
-      </c>
-      <c r="C9" s="0">
+      <c r="B9" s="1">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1">
         <v>140.59883117675781</v>
       </c>
     </row>
@@ -243,10 +245,10 @@
       <c r="A10" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="0">
-        <v>9</v>
-      </c>
-      <c r="C10" s="0">
+      <c r="B10" s="1">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1">
         <v>193.86285400390625</v>
       </c>
     </row>
@@ -254,21 +256,21 @@
       <c r="A11" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="0">
-        <v>10</v>
-      </c>
-      <c r="C11" s="0">
-        <v>256.06808471679687</v>
+      <c r="B11" s="1">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1">
+        <v>256.06808471679688</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="0">
-        <v>11</v>
-      </c>
-      <c r="C12" s="0">
+      <c r="B12" s="1">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1">
         <v>172.85871887207031</v>
       </c>
     </row>
@@ -276,10 +278,10 @@
       <c r="A13" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="0">
-        <v>12</v>
-      </c>
-      <c r="C13" s="0">
+      <c r="B13" s="1">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1">
         <v>123.54463195800781</v>
       </c>
     </row>
@@ -287,10 +289,10 @@
       <c r="A14" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="0">
-        <v>1</v>
-      </c>
-      <c r="C14" s="0">
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
         <v>99.624839782714844</v>
       </c>
     </row>
@@ -298,10 +300,10 @@
       <c r="A15" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="0">
-        <v>2</v>
-      </c>
-      <c r="C15" s="0">
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1">
         <v>89.3013916015625</v>
       </c>
     </row>
@@ -309,10 +311,10 @@
       <c r="A16" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="0">
-        <v>3</v>
-      </c>
-      <c r="C16" s="0">
+      <c r="B16" s="1">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1">
         <v>84.704429626464844</v>
       </c>
     </row>
@@ -320,10 +322,10 @@
       <c r="A17" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="0">
-        <v>4</v>
-      </c>
-      <c r="C17" s="0">
+      <c r="B17" s="1">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1">
         <v>63.930248260498047</v>
       </c>
     </row>
@@ -331,21 +333,21 @@
       <c r="A18" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="0">
-        <v>5</v>
-      </c>
-      <c r="C18" s="0">
-        <v>71.887985229492187</v>
+      <c r="B18" s="1">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1">
+        <v>71.887985229492188</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="0">
-        <v>6</v>
-      </c>
-      <c r="C19" s="0">
+      <c r="B19" s="1">
+        <v>6</v>
+      </c>
+      <c r="C19" s="1">
         <v>52.256729125976563</v>
       </c>
     </row>
@@ -353,10 +355,10 @@
       <c r="A20" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="0">
-        <v>7</v>
-      </c>
-      <c r="C20" s="0">
+      <c r="B20" s="1">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1">
         <v>81.232292175292969</v>
       </c>
     </row>
@@ -364,10 +366,10 @@
       <c r="A21" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="0">
-        <v>8</v>
-      </c>
-      <c r="C21" s="0">
+      <c r="B21" s="1">
+        <v>8</v>
+      </c>
+      <c r="C21" s="1">
         <v>72.576705932617188</v>
       </c>
     </row>
@@ -375,10 +377,10 @@
       <c r="A22" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="0">
-        <v>9</v>
-      </c>
-      <c r="C22" s="0">
+      <c r="B22" s="1">
+        <v>9</v>
+      </c>
+      <c r="C22" s="1">
         <v>67.1275634765625</v>
       </c>
     </row>
@@ -386,10 +388,10 @@
       <c r="A23" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="0">
-        <v>10</v>
-      </c>
-      <c r="C23" s="0">
+      <c r="B23" s="1">
+        <v>10</v>
+      </c>
+      <c r="C23" s="1">
         <v>123.12413024902344</v>
       </c>
     </row>
@@ -397,10 +399,10 @@
       <c r="A24" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="0">
-        <v>11</v>
-      </c>
-      <c r="C24" s="0">
+      <c r="B24" s="1">
+        <v>11</v>
+      </c>
+      <c r="C24" s="1">
         <v>26.846799850463867</v>
       </c>
     </row>
@@ -408,10 +410,10 @@
       <c r="A25" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="0">
-        <v>12</v>
-      </c>
-      <c r="C25" s="0">
+      <c r="B25" s="1">
+        <v>12</v>
+      </c>
+      <c r="C25" s="1">
         <v>48.689983367919922</v>
       </c>
     </row>
@@ -419,10 +421,10 @@
       <c r="A26" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="0">
-        <v>1</v>
-      </c>
-      <c r="C26" s="0">
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1">
         <v>53.748451232910156</v>
       </c>
     </row>
@@ -430,10 +432,10 @@
       <c r="A27" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="0">
-        <v>2</v>
-      </c>
-      <c r="C27" s="0">
+      <c r="B27" s="1">
+        <v>2</v>
+      </c>
+      <c r="C27" s="1">
         <v>58.396511077880859</v>
       </c>
     </row>
@@ -441,10 +443,10 @@
       <c r="A28" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="0">
-        <v>3</v>
-      </c>
-      <c r="C28" s="0">
+      <c r="B28" s="1">
+        <v>3</v>
+      </c>
+      <c r="C28" s="1">
         <v>61.960391998291016</v>
       </c>
     </row>
@@ -452,10 +454,10 @@
       <c r="A29" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="0">
-        <v>4</v>
-      </c>
-      <c r="C29" s="0">
+      <c r="B29" s="1">
+        <v>4</v>
+      </c>
+      <c r="C29" s="1">
         <v>114.01042938232422</v>
       </c>
     </row>
@@ -463,10 +465,10 @@
       <c r="A30" t="s">
         <v>3</v>
       </c>
-      <c r="B30" s="0">
-        <v>5</v>
-      </c>
-      <c r="C30" s="0">
+      <c r="B30" s="1">
+        <v>5</v>
+      </c>
+      <c r="C30" s="1">
         <v>46.368324279785156</v>
       </c>
     </row>
@@ -474,21 +476,21 @@
       <c r="A31" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="0">
-        <v>6</v>
-      </c>
-      <c r="C31" s="0">
-        <v>133.21640014648437</v>
+      <c r="B31" s="1">
+        <v>6</v>
+      </c>
+      <c r="C31" s="1">
+        <v>133.21640014648438</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="0">
-        <v>7</v>
-      </c>
-      <c r="C32" s="0">
+      <c r="B32" s="1">
+        <v>7</v>
+      </c>
+      <c r="C32" s="1">
         <v>73.706695556640625</v>
       </c>
     </row>
@@ -496,10 +498,10 @@
       <c r="A33" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="0">
-        <v>8</v>
-      </c>
-      <c r="C33" s="0">
+      <c r="B33" s="1">
+        <v>8</v>
+      </c>
+      <c r="C33" s="1">
         <v>42.748378753662109</v>
       </c>
     </row>
@@ -507,10 +509,10 @@
       <c r="A34" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="0">
-        <v>9</v>
-      </c>
-      <c r="C34" s="0">
+      <c r="B34" s="1">
+        <v>9</v>
+      </c>
+      <c r="C34" s="1">
         <v>55.577869415283203</v>
       </c>
     </row>
@@ -518,10 +520,10 @@
       <c r="A35" t="s">
         <v>3</v>
       </c>
-      <c r="B35" s="0">
-        <v>10</v>
-      </c>
-      <c r="C35" s="0">
+      <c r="B35" s="1">
+        <v>10</v>
+      </c>
+      <c r="C35" s="1">
         <v>55.821765899658203</v>
       </c>
     </row>
@@ -529,10 +531,10 @@
       <c r="A36" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="0">
-        <v>11</v>
-      </c>
-      <c r="C36" s="0">
+      <c r="B36" s="1">
+        <v>11</v>
+      </c>
+      <c r="C36" s="1">
         <v>68.99102783203125</v>
       </c>
     </row>
@@ -540,10 +542,10 @@
       <c r="A37" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="0">
-        <v>12</v>
-      </c>
-      <c r="C37" s="0">
+      <c r="B37" s="1">
+        <v>12</v>
+      </c>
+      <c r="C37" s="1">
         <v>66.450172424316406</v>
       </c>
     </row>
@@ -551,10 +553,10 @@
       <c r="A38" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="0">
-        <v>1</v>
-      </c>
-      <c r="C38" s="0">
+      <c r="B38" s="1">
+        <v>1</v>
+      </c>
+      <c r="C38" s="1">
         <v>38.407833099365234</v>
       </c>
     </row>
@@ -562,10 +564,10 @@
       <c r="A39" t="s">
         <v>4</v>
       </c>
-      <c r="B39" s="0">
-        <v>2</v>
-      </c>
-      <c r="C39" s="0">
+      <c r="B39" s="1">
+        <v>2</v>
+      </c>
+      <c r="C39" s="1">
         <v>56.693271636962891</v>
       </c>
     </row>
@@ -573,10 +575,10 @@
       <c r="A40" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="0">
-        <v>3</v>
-      </c>
-      <c r="C40" s="0">
+      <c r="B40" s="1">
+        <v>3</v>
+      </c>
+      <c r="C40" s="1">
         <v>91.642860412597656</v>
       </c>
     </row>
@@ -584,10 +586,10 @@
       <c r="A41" t="s">
         <v>4</v>
       </c>
-      <c r="B41" s="0">
-        <v>4</v>
-      </c>
-      <c r="C41" s="0">
+      <c r="B41" s="1">
+        <v>4</v>
+      </c>
+      <c r="C41" s="1">
         <v>100.98927307128906</v>
       </c>
     </row>
@@ -595,10 +597,10 @@
       <c r="A42" t="s">
         <v>4</v>
       </c>
-      <c r="B42" s="0">
-        <v>5</v>
-      </c>
-      <c r="C42" s="0">
+      <c r="B42" s="1">
+        <v>5</v>
+      </c>
+      <c r="C42" s="1">
         <v>98.2562255859375</v>
       </c>
     </row>
@@ -606,10 +608,10 @@
       <c r="A43" t="s">
         <v>4</v>
       </c>
-      <c r="B43" s="0">
-        <v>6</v>
-      </c>
-      <c r="C43" s="0">
+      <c r="B43" s="1">
+        <v>6</v>
+      </c>
+      <c r="C43" s="1">
         <v>74.842735290527344</v>
       </c>
     </row>
@@ -617,10 +619,10 @@
       <c r="A44" t="s">
         <v>4</v>
       </c>
-      <c r="B44" s="0">
-        <v>7</v>
-      </c>
-      <c r="C44" s="0">
+      <c r="B44" s="1">
+        <v>7</v>
+      </c>
+      <c r="C44" s="1">
         <v>66.38372802734375</v>
       </c>
     </row>
@@ -628,10 +630,10 @@
       <c r="A45" t="s">
         <v>4</v>
       </c>
-      <c r="B45" s="0">
-        <v>8</v>
-      </c>
-      <c r="C45" s="0">
+      <c r="B45" s="1">
+        <v>8</v>
+      </c>
+      <c r="C45" s="1">
         <v>105.13270568847656</v>
       </c>
     </row>
@@ -639,10 +641,10 @@
       <c r="A46" t="s">
         <v>4</v>
       </c>
-      <c r="B46" s="0">
-        <v>9</v>
-      </c>
-      <c r="C46" s="0">
+      <c r="B46" s="1">
+        <v>9</v>
+      </c>
+      <c r="C46" s="1">
         <v>205.25697326660156</v>
       </c>
     </row>
@@ -650,10 +652,10 @@
       <c r="A47" t="s">
         <v>4</v>
       </c>
-      <c r="B47" s="0">
-        <v>10</v>
-      </c>
-      <c r="C47" s="0">
+      <c r="B47" s="1">
+        <v>10</v>
+      </c>
+      <c r="C47" s="1">
         <v>158.72160339355469</v>
       </c>
     </row>
@@ -661,10 +663,10 @@
       <c r="A48" t="s">
         <v>4</v>
       </c>
-      <c r="B48" s="0">
-        <v>11</v>
-      </c>
-      <c r="C48" s="0">
+      <c r="B48" s="1">
+        <v>11</v>
+      </c>
+      <c r="C48" s="1">
         <v>146.11531066894531</v>
       </c>
     </row>
@@ -672,10 +674,10 @@
       <c r="A49" t="s">
         <v>4</v>
       </c>
-      <c r="B49" s="0">
-        <v>12</v>
-      </c>
-      <c r="C49" s="0">
+      <c r="B49" s="1">
+        <v>12</v>
+      </c>
+      <c r="C49" s="1">
         <v>108.11412811279297</v>
       </c>
     </row>
@@ -683,10 +685,10 @@
       <c r="A50" t="s">
         <v>5</v>
       </c>
-      <c r="B50" s="0">
-        <v>1</v>
-      </c>
-      <c r="C50" s="0">
+      <c r="B50" s="1">
+        <v>1</v>
+      </c>
+      <c r="C50" s="1">
         <v>85.506576538085938</v>
       </c>
     </row>
@@ -694,10 +696,10 @@
       <c r="A51" t="s">
         <v>5</v>
       </c>
-      <c r="B51" s="0">
-        <v>2</v>
-      </c>
-      <c r="C51" s="0">
+      <c r="B51" s="1">
+        <v>2</v>
+      </c>
+      <c r="C51" s="1">
         <v>70.793487548828125</v>
       </c>
     </row>
@@ -705,10 +707,10 @@
       <c r="A52" t="s">
         <v>5</v>
       </c>
-      <c r="B52" s="0">
-        <v>3</v>
-      </c>
-      <c r="C52" s="0">
+      <c r="B52" s="1">
+        <v>3</v>
+      </c>
+      <c r="C52" s="1">
         <v>76.328315734863281</v>
       </c>
     </row>
@@ -716,10 +718,10 @@
       <c r="A53" t="s">
         <v>5</v>
       </c>
-      <c r="B53" s="0">
-        <v>4</v>
-      </c>
-      <c r="C53" s="0">
+      <c r="B53" s="1">
+        <v>4</v>
+      </c>
+      <c r="C53" s="1">
         <v>78.088180541992188</v>
       </c>
     </row>
@@ -727,10 +729,10 @@
       <c r="A54" t="s">
         <v>5</v>
       </c>
-      <c r="B54" s="0">
-        <v>5</v>
-      </c>
-      <c r="C54" s="0">
+      <c r="B54" s="1">
+        <v>5</v>
+      </c>
+      <c r="C54" s="1">
         <v>67.406356811523438</v>
       </c>
     </row>
@@ -738,10 +740,10 @@
       <c r="A55" t="s">
         <v>5</v>
       </c>
-      <c r="B55" s="0">
-        <v>6</v>
-      </c>
-      <c r="C55" s="0">
+      <c r="B55" s="1">
+        <v>6</v>
+      </c>
+      <c r="C55" s="1">
         <v>86.87921142578125</v>
       </c>
     </row>
@@ -749,10 +751,10 @@
       <c r="A56" t="s">
         <v>5</v>
       </c>
-      <c r="B56" s="0">
-        <v>7</v>
-      </c>
-      <c r="C56" s="0">
+      <c r="B56" s="1">
+        <v>7</v>
+      </c>
+      <c r="C56" s="1">
         <v>88.472572326660156</v>
       </c>
     </row>
@@ -760,10 +762,10 @@
       <c r="A57" t="s">
         <v>5</v>
       </c>
-      <c r="B57" s="0">
-        <v>8</v>
-      </c>
-      <c r="C57" s="0">
+      <c r="B57" s="1">
+        <v>8</v>
+      </c>
+      <c r="C57" s="1">
         <v>93.7239990234375</v>
       </c>
     </row>
@@ -771,10 +773,10 @@
       <c r="A58" t="s">
         <v>5</v>
       </c>
-      <c r="B58" s="0">
-        <v>9</v>
-      </c>
-      <c r="C58" s="0">
+      <c r="B58" s="1">
+        <v>9</v>
+      </c>
+      <c r="C58" s="1">
         <v>127.27272796630859</v>
       </c>
     </row>
@@ -782,10 +784,10 @@
       <c r="A59" t="s">
         <v>5</v>
       </c>
-      <c r="B59" s="0">
-        <v>10</v>
-      </c>
-      <c r="C59" s="0">
+      <c r="B59" s="1">
+        <v>10</v>
+      </c>
+      <c r="C59" s="1">
         <v>108.42975616455078</v>
       </c>
     </row>
@@ -793,10 +795,10 @@
       <c r="A60" t="s">
         <v>5</v>
       </c>
-      <c r="B60" s="0">
-        <v>11</v>
-      </c>
-      <c r="C60" s="0">
+      <c r="B60" s="1">
+        <v>11</v>
+      </c>
+      <c r="C60" s="1">
         <v>115.09958648681641</v>
       </c>
     </row>
@@ -804,10 +806,10 @@
       <c r="A61" t="s">
         <v>5</v>
       </c>
-      <c r="B61" s="0">
-        <v>12</v>
-      </c>
-      <c r="C61" s="0">
+      <c r="B61" s="1">
+        <v>12</v>
+      </c>
+      <c r="C61" s="1">
         <v>118.64259338378906</v>
       </c>
     </row>
@@ -815,32 +817,32 @@
       <c r="A62" t="s">
         <v>6</v>
       </c>
-      <c r="B62" s="0">
-        <v>1</v>
-      </c>
-      <c r="C62" s="0">
-        <v>146.05941772460937</v>
+      <c r="B62" s="1">
+        <v>1</v>
+      </c>
+      <c r="C62" s="1">
+        <v>146.05941772460938</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
         <v>6</v>
       </c>
-      <c r="B63" s="0">
-        <v>2</v>
-      </c>
-      <c r="C63" s="0">
-        <v>178.73886108398437</v>
+      <c r="B63" s="1">
+        <v>2</v>
+      </c>
+      <c r="C63" s="1">
+        <v>178.73886108398438</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
         <v>6</v>
       </c>
-      <c r="B64" s="0">
-        <v>3</v>
-      </c>
-      <c r="C64" s="0">
+      <c r="B64" s="1">
+        <v>3</v>
+      </c>
+      <c r="C64" s="1">
         <v>174.97273254394531</v>
       </c>
     </row>
@@ -848,21 +850,21 @@
       <c r="A65" t="s">
         <v>6</v>
       </c>
-      <c r="B65" s="0">
-        <v>4</v>
-      </c>
-      <c r="C65" s="0">
-        <v>153.50643920898437</v>
+      <c r="B65" s="1">
+        <v>4</v>
+      </c>
+      <c r="C65" s="1">
+        <v>153.50643920898438</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
         <v>6</v>
       </c>
-      <c r="B66" s="0">
-        <v>5</v>
-      </c>
-      <c r="C66" s="0">
+      <c r="B66" s="1">
+        <v>5</v>
+      </c>
+      <c r="C66" s="1">
         <v>93.713760375976563</v>
       </c>
     </row>
@@ -870,10 +872,10 @@
       <c r="A67" t="s">
         <v>6</v>
       </c>
-      <c r="B67" s="0">
-        <v>6</v>
-      </c>
-      <c r="C67" s="0">
+      <c r="B67" s="1">
+        <v>6</v>
+      </c>
+      <c r="C67" s="1">
         <v>125.0064697265625</v>
       </c>
     </row>
@@ -881,10 +883,10 @@
       <c r="A68" t="s">
         <v>6</v>
       </c>
-      <c r="B68" s="0">
-        <v>7</v>
-      </c>
-      <c r="C68" s="0">
+      <c r="B68" s="1">
+        <v>7</v>
+      </c>
+      <c r="C68" s="1">
         <v>80.936637878417969</v>
       </c>
     </row>
@@ -892,10 +894,10 @@
       <c r="A69" t="s">
         <v>6</v>
       </c>
-      <c r="B69" s="0">
-        <v>8</v>
-      </c>
-      <c r="C69" s="0">
+      <c r="B69" s="1">
+        <v>8</v>
+      </c>
+      <c r="C69" s="1">
         <v>83.362625122070313</v>
       </c>
     </row>
@@ -903,10 +905,10 @@
       <c r="A70" t="s">
         <v>6</v>
       </c>
-      <c r="B70" s="0">
-        <v>9</v>
-      </c>
-      <c r="C70" s="0">
+      <c r="B70" s="1">
+        <v>9</v>
+      </c>
+      <c r="C70" s="1">
         <v>65.412857055664063</v>
       </c>
     </row>
@@ -914,10 +916,10 @@
       <c r="A71" t="s">
         <v>6</v>
       </c>
-      <c r="B71" s="0">
-        <v>10</v>
-      </c>
-      <c r="C71" s="0">
+      <c r="B71" s="1">
+        <v>10</v>
+      </c>
+      <c r="C71" s="1">
         <v>62.298290252685547</v>
       </c>
     </row>
@@ -925,10 +927,10 @@
       <c r="A72" t="s">
         <v>6</v>
       </c>
-      <c r="B72" s="0">
-        <v>11</v>
-      </c>
-      <c r="C72" s="0">
+      <c r="B72" s="1">
+        <v>11</v>
+      </c>
+      <c r="C72" s="1">
         <v>78.4478759765625</v>
       </c>
     </row>
@@ -936,10 +938,10 @@
       <c r="A73" t="s">
         <v>6</v>
       </c>
-      <c r="B73" s="0">
-        <v>12</v>
-      </c>
-      <c r="C73" s="0">
+      <c r="B73" s="1">
+        <v>12</v>
+      </c>
+      <c r="C73" s="1">
         <v>46.291194915771484</v>
       </c>
     </row>
@@ -947,10 +949,10 @@
       <c r="A74" t="s">
         <v>7</v>
       </c>
-      <c r="B74" s="0">
-        <v>1</v>
-      </c>
-      <c r="C74" s="0">
+      <c r="B74" s="1">
+        <v>1</v>
+      </c>
+      <c r="C74" s="1">
         <v>24.035942077636719</v>
       </c>
     </row>
@@ -958,10 +960,10 @@
       <c r="A75" t="s">
         <v>7</v>
       </c>
-      <c r="B75" s="0">
-        <v>2</v>
-      </c>
-      <c r="C75" s="0">
+      <c r="B75" s="1">
+        <v>2</v>
+      </c>
+      <c r="C75" s="1">
         <v>57.130153656005859</v>
       </c>
     </row>
@@ -969,10 +971,10 @@
       <c r="A76" t="s">
         <v>7</v>
       </c>
-      <c r="B76" s="0">
-        <v>3</v>
-      </c>
-      <c r="C76" s="0">
+      <c r="B76" s="1">
+        <v>3</v>
+      </c>
+      <c r="C76" s="1">
         <v>61.884700775146484</v>
       </c>
     </row>
@@ -980,10 +982,10 @@
       <c r="A77" t="s">
         <v>7</v>
       </c>
-      <c r="B77" s="0">
-        <v>4</v>
-      </c>
-      <c r="C77" s="0">
+      <c r="B77" s="1">
+        <v>4</v>
+      </c>
+      <c r="C77" s="1">
         <v>38.552352905273438</v>
       </c>
     </row>
@@ -991,10 +993,10 @@
       <c r="A78" t="s">
         <v>7</v>
       </c>
-      <c r="B78" s="0">
-        <v>5</v>
-      </c>
-      <c r="C78" s="0">
+      <c r="B78" s="1">
+        <v>5</v>
+      </c>
+      <c r="C78" s="1">
         <v>42.882164001464844</v>
       </c>
     </row>
@@ -1002,10 +1004,10 @@
       <c r="A79" t="s">
         <v>7</v>
       </c>
-      <c r="B79" s="0">
-        <v>6</v>
-      </c>
-      <c r="C79" s="0">
+      <c r="B79" s="1">
+        <v>6</v>
+      </c>
+      <c r="C79" s="1">
         <v>49.439136505126953</v>
       </c>
     </row>
@@ -1013,10 +1015,10 @@
       <c r="A80" t="s">
         <v>7</v>
       </c>
-      <c r="B80" s="0">
-        <v>7</v>
-      </c>
-      <c r="C80" s="0">
+      <c r="B80" s="1">
+        <v>7</v>
+      </c>
+      <c r="C80" s="1">
         <v>52.617275238037109</v>
       </c>
     </row>
@@ -1024,10 +1026,10 @@
       <c r="A81" t="s">
         <v>7</v>
       </c>
-      <c r="B81" s="0">
-        <v>8</v>
-      </c>
-      <c r="C81" s="0">
+      <c r="B81" s="1">
+        <v>8</v>
+      </c>
+      <c r="C81" s="1">
         <v>39.393718719482422</v>
       </c>
     </row>
@@ -1035,10 +1037,10 @@
       <c r="A82" t="s">
         <v>7</v>
       </c>
-      <c r="B82" s="0">
-        <v>9</v>
-      </c>
-      <c r="C82" s="0">
+      <c r="B82" s="1">
+        <v>9</v>
+      </c>
+      <c r="C82" s="1">
         <v>49.166225433349609</v>
       </c>
     </row>
@@ -1046,10 +1048,10 @@
       <c r="A83" t="s">
         <v>7</v>
       </c>
-      <c r="B83" s="0">
-        <v>10</v>
-      </c>
-      <c r="C83" s="0">
+      <c r="B83" s="1">
+        <v>10</v>
+      </c>
+      <c r="C83" s="1">
         <v>67.129158020019531</v>
       </c>
     </row>
@@ -1057,10 +1059,10 @@
       <c r="A84" t="s">
         <v>7</v>
       </c>
-      <c r="B84" s="0">
-        <v>11</v>
-      </c>
-      <c r="C84" s="0">
+      <c r="B84" s="1">
+        <v>11</v>
+      </c>
+      <c r="C84" s="1">
         <v>68.726028442382813</v>
       </c>
     </row>
@@ -1068,10 +1070,10 @@
       <c r="A85" t="s">
         <v>7</v>
       </c>
-      <c r="B85" s="0">
-        <v>12</v>
-      </c>
-      <c r="C85" s="0">
+      <c r="B85" s="1">
+        <v>12</v>
+      </c>
+      <c r="C85" s="1">
         <v>44.909515380859375</v>
       </c>
     </row>
@@ -1079,10 +1081,10 @@
       <c r="A86" t="s">
         <v>8</v>
       </c>
-      <c r="B86" s="0">
-        <v>1</v>
-      </c>
-      <c r="C86" s="0">
+      <c r="B86" s="1">
+        <v>1</v>
+      </c>
+      <c r="C86" s="1">
         <v>43.989646911621094</v>
       </c>
     </row>
@@ -1090,10 +1092,10 @@
       <c r="A87" t="s">
         <v>8</v>
       </c>
-      <c r="B87" s="0">
-        <v>2</v>
-      </c>
-      <c r="C87" s="0">
+      <c r="B87" s="1">
+        <v>2</v>
+      </c>
+      <c r="C87" s="1">
         <v>39.645351409912109</v>
       </c>
     </row>
@@ -1101,10 +1103,10 @@
       <c r="A88" t="s">
         <v>8</v>
       </c>
-      <c r="B88" s="0">
-        <v>3</v>
-      </c>
-      <c r="C88" s="0">
+      <c r="B88" s="1">
+        <v>3</v>
+      </c>
+      <c r="C88" s="1">
         <v>34.078708648681641</v>
       </c>
     </row>
@@ -1112,10 +1114,10 @@
       <c r="A89" t="s">
         <v>8</v>
       </c>
-      <c r="B89" s="0">
-        <v>4</v>
-      </c>
-      <c r="C89" s="0">
+      <c r="B89" s="1">
+        <v>4</v>
+      </c>
+      <c r="C89" s="1">
         <v>69.05712890625</v>
       </c>
     </row>
@@ -1123,10 +1125,10 @@
       <c r="A90" t="s">
         <v>8</v>
       </c>
-      <c r="B90" s="0">
-        <v>5</v>
-      </c>
-      <c r="C90" s="0">
+      <c r="B90" s="1">
+        <v>5</v>
+      </c>
+      <c r="C90" s="1">
         <v>71.771087646484375</v>
       </c>
     </row>
@@ -1134,10 +1136,10 @@
       <c r="A91" t="s">
         <v>8</v>
       </c>
-      <c r="B91" s="0">
-        <v>6</v>
-      </c>
-      <c r="C91" s="0">
+      <c r="B91" s="1">
+        <v>6</v>
+      </c>
+      <c r="C91" s="1">
         <v>59.403873443603516</v>
       </c>
     </row>
@@ -1145,10 +1147,10 @@
       <c r="A92" t="s">
         <v>8</v>
       </c>
-      <c r="B92" s="0">
-        <v>7</v>
-      </c>
-      <c r="C92" s="0">
+      <c r="B92" s="1">
+        <v>7</v>
+      </c>
+      <c r="C92" s="1">
         <v>47.414012908935547</v>
       </c>
     </row>
@@ -1156,10 +1158,10 @@
       <c r="A93" t="s">
         <v>8</v>
       </c>
-      <c r="B93" s="0">
-        <v>8</v>
-      </c>
-      <c r="C93" s="0">
+      <c r="B93" s="1">
+        <v>8</v>
+      </c>
+      <c r="C93" s="1">
         <v>48.541706085205078</v>
       </c>
     </row>
@@ -1167,10 +1169,10 @@
       <c r="A94" t="s">
         <v>8</v>
       </c>
-      <c r="B94" s="0">
-        <v>9</v>
-      </c>
-      <c r="C94" s="0">
+      <c r="B94" s="1">
+        <v>9</v>
+      </c>
+      <c r="C94" s="1">
         <v>70.332473754882813</v>
       </c>
     </row>
@@ -1178,10 +1180,10 @@
       <c r="A95" t="s">
         <v>8</v>
       </c>
-      <c r="B95" s="0">
-        <v>10</v>
-      </c>
-      <c r="C95" s="0">
+      <c r="B95" s="1">
+        <v>10</v>
+      </c>
+      <c r="C95" s="1">
         <v>40.613033294677734</v>
       </c>
     </row>
@@ -1189,10 +1191,10 @@
       <c r="A96" t="s">
         <v>8</v>
       </c>
-      <c r="B96" s="0">
-        <v>11</v>
-      </c>
-      <c r="C96" s="0">
+      <c r="B96" s="1">
+        <v>11</v>
+      </c>
+      <c r="C96" s="1">
         <v>47.559238433837891</v>
       </c>
     </row>
@@ -1200,10 +1202,10 @@
       <c r="A97" t="s">
         <v>8</v>
       </c>
-      <c r="B97" s="0">
-        <v>12</v>
-      </c>
-      <c r="C97" s="0">
+      <c r="B97" s="1">
+        <v>12</v>
+      </c>
+      <c r="C97" s="1">
         <v>33.106582641601563</v>
       </c>
     </row>
@@ -1211,10 +1213,10 @@
       <c r="A98" t="s">
         <v>9</v>
       </c>
-      <c r="B98" s="0">
-        <v>1</v>
-      </c>
-      <c r="C98" s="0">
+      <c r="B98" s="1">
+        <v>1</v>
+      </c>
+      <c r="C98" s="1">
         <v>44.040050506591797</v>
       </c>
     </row>
@@ -1222,10 +1224,10 @@
       <c r="A99" t="s">
         <v>9</v>
       </c>
-      <c r="B99" s="0">
-        <v>2</v>
-      </c>
-      <c r="C99" s="0">
+      <c r="B99" s="1">
+        <v>2</v>
+      </c>
+      <c r="C99" s="1">
         <v>37.132061004638672</v>
       </c>
     </row>
@@ -1233,10 +1235,10 @@
       <c r="A100" t="s">
         <v>9</v>
       </c>
-      <c r="B100" s="0">
-        <v>3</v>
-      </c>
-      <c r="C100" s="0">
+      <c r="B100" s="1">
+        <v>3</v>
+      </c>
+      <c r="C100" s="1">
         <v>42.456447601318359</v>
       </c>
     </row>
@@ -1244,10 +1246,10 @@
       <c r="A101" t="s">
         <v>9</v>
       </c>
-      <c r="B101" s="0">
-        <v>4</v>
-      </c>
-      <c r="C101" s="0">
+      <c r="B101" s="1">
+        <v>4</v>
+      </c>
+      <c r="C101" s="1">
         <v>37.08660888671875</v>
       </c>
     </row>
@@ -1255,10 +1257,10 @@
       <c r="A102" t="s">
         <v>9</v>
       </c>
-      <c r="B102" s="0">
-        <v>5</v>
-      </c>
-      <c r="C102" s="0">
+      <c r="B102" s="1">
+        <v>5</v>
+      </c>
+      <c r="C102" s="1">
         <v>74.022674560546875</v>
       </c>
     </row>
@@ -1266,10 +1268,10 @@
       <c r="A103" t="s">
         <v>9</v>
       </c>
-      <c r="B103" s="0">
-        <v>6</v>
-      </c>
-      <c r="C103" s="0">
+      <c r="B103" s="1">
+        <v>6</v>
+      </c>
+      <c r="C103" s="1">
         <v>59.820568084716797</v>
       </c>
     </row>
@@ -1277,10 +1279,10 @@
       <c r="A104" t="s">
         <v>9</v>
       </c>
-      <c r="B104" s="0">
-        <v>7</v>
-      </c>
-      <c r="C104" s="0">
+      <c r="B104" s="1">
+        <v>7</v>
+      </c>
+      <c r="C104" s="1">
         <v>47.543785095214844</v>
       </c>
     </row>
@@ -1288,10 +1290,10 @@
       <c r="A105" t="s">
         <v>9</v>
       </c>
-      <c r="B105" s="0">
-        <v>8</v>
-      </c>
-      <c r="C105" s="0">
+      <c r="B105" s="1">
+        <v>8</v>
+      </c>
+      <c r="C105" s="1">
         <v>67.213226318359375</v>
       </c>
     </row>
@@ -1299,10 +1301,10 @@
       <c r="A106" t="s">
         <v>9</v>
       </c>
-      <c r="B106" s="0">
-        <v>9</v>
-      </c>
-      <c r="C106" s="0">
+      <c r="B106" s="1">
+        <v>9</v>
+      </c>
+      <c r="C106" s="1">
         <v>56.234481811523438</v>
       </c>
     </row>
@@ -1310,21 +1312,21 @@
       <c r="A107" t="s">
         <v>9</v>
       </c>
-      <c r="B107" s="0">
-        <v>10</v>
-      </c>
-      <c r="C107" s="0">
-        <v>65.255081176757812</v>
+      <c r="B107" s="1">
+        <v>10</v>
+      </c>
+      <c r="C107" s="1">
+        <v>65.255081176757813</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
         <v>9</v>
       </c>
-      <c r="B108" s="0">
-        <v>11</v>
-      </c>
-      <c r="C108" s="0">
+      <c r="B108" s="1">
+        <v>11</v>
+      </c>
+      <c r="C108" s="1">
         <v>59.490592956542969</v>
       </c>
     </row>
@@ -1332,10 +1334,10 @@
       <c r="A109" t="s">
         <v>9</v>
       </c>
-      <c r="B109" s="0">
-        <v>12</v>
-      </c>
-      <c r="C109" s="0">
+      <c r="B109" s="1">
+        <v>12</v>
+      </c>
+      <c r="C109" s="1">
         <v>64.488700866699219</v>
       </c>
     </row>
@@ -1343,10 +1345,10 @@
       <c r="A110" t="s">
         <v>10</v>
       </c>
-      <c r="B110" s="0">
-        <v>1</v>
-      </c>
-      <c r="C110" s="0">
+      <c r="B110" s="1">
+        <v>1</v>
+      </c>
+      <c r="C110" s="1">
         <v>49.232185363769531</v>
       </c>
     </row>
@@ -1354,10 +1356,10 @@
       <c r="A111" t="s">
         <v>10</v>
       </c>
-      <c r="B111" s="0">
-        <v>2</v>
-      </c>
-      <c r="C111" s="0">
+      <c r="B111" s="1">
+        <v>2</v>
+      </c>
+      <c r="C111" s="1">
         <v>53.071933746337891</v>
       </c>
     </row>
@@ -1365,10 +1367,10 @@
       <c r="A112" t="s">
         <v>10</v>
       </c>
-      <c r="B112" s="0">
-        <v>3</v>
-      </c>
-      <c r="C112" s="0">
+      <c r="B112" s="1">
+        <v>3</v>
+      </c>
+      <c r="C112" s="1">
         <v>77.055221557617188</v>
       </c>
     </row>
@@ -1376,10 +1378,10 @@
       <c r="A113" t="s">
         <v>10</v>
       </c>
-      <c r="B113" s="0">
-        <v>4</v>
-      </c>
-      <c r="C113" s="0">
+      <c r="B113" s="1">
+        <v>4</v>
+      </c>
+      <c r="C113" s="1">
         <v>60.96484375</v>
       </c>
     </row>
@@ -1387,10 +1389,10 @@
       <c r="A114" t="s">
         <v>10</v>
       </c>
-      <c r="B114" s="0">
-        <v>5</v>
-      </c>
-      <c r="C114" s="0">
+      <c r="B114" s="1">
+        <v>5</v>
+      </c>
+      <c r="C114" s="1">
         <v>66.573944091796875</v>
       </c>
     </row>
@@ -1398,10 +1400,10 @@
       <c r="A115" t="s">
         <v>10</v>
       </c>
-      <c r="B115" s="0">
-        <v>6</v>
-      </c>
-      <c r="C115" s="0">
+      <c r="B115" s="1">
+        <v>6</v>
+      </c>
+      <c r="C115" s="1">
         <v>53.468608856201172</v>
       </c>
     </row>
@@ -1409,10 +1411,10 @@
       <c r="A116" t="s">
         <v>10</v>
       </c>
-      <c r="B116" s="0">
-        <v>7</v>
-      </c>
-      <c r="C116" s="0">
+      <c r="B116" s="1">
+        <v>7</v>
+      </c>
+      <c r="C116" s="1">
         <v>48.757678985595703</v>
       </c>
     </row>
@@ -1420,10 +1422,10 @@
       <c r="A117" t="s">
         <v>10</v>
       </c>
-      <c r="B117" s="0">
-        <v>8</v>
-      </c>
-      <c r="C117" s="0">
+      <c r="B117" s="1">
+        <v>8</v>
+      </c>
+      <c r="C117" s="1">
         <v>77.388679504394531</v>
       </c>
     </row>
@@ -1431,10 +1433,10 @@
       <c r="A118" t="s">
         <v>10</v>
       </c>
-      <c r="B118" s="0">
-        <v>9</v>
-      </c>
-      <c r="C118" s="0">
+      <c r="B118" s="1">
+        <v>9</v>
+      </c>
+      <c r="C118" s="1">
         <v>132.26576232910156</v>
       </c>
     </row>
@@ -1442,10 +1444,10 @@
       <c r="A119" t="s">
         <v>10</v>
       </c>
-      <c r="B119" s="0">
-        <v>10</v>
-      </c>
-      <c r="C119" s="0">
+      <c r="B119" s="1">
+        <v>10</v>
+      </c>
+      <c r="C119" s="1">
         <v>91.692916870117188</v>
       </c>
     </row>
@@ -1453,10 +1455,10 @@
       <c r="A120" t="s">
         <v>10</v>
       </c>
-      <c r="B120" s="0">
-        <v>11</v>
-      </c>
-      <c r="C120" s="0">
+      <c r="B120" s="1">
+        <v>11</v>
+      </c>
+      <c r="C120" s="1">
         <v>131.62321472167969</v>
       </c>
     </row>
@@ -1464,10 +1466,10 @@
       <c r="A121" t="s">
         <v>10</v>
       </c>
-      <c r="B121" s="0">
-        <v>12</v>
-      </c>
-      <c r="C121" s="0">
+      <c r="B121" s="1">
+        <v>12</v>
+      </c>
+      <c r="C121" s="1">
         <v>150.87321472167969</v>
       </c>
     </row>
@@ -1475,10 +1477,10 @@
       <c r="A122" t="s">
         <v>11</v>
       </c>
-      <c r="B122" s="0">
-        <v>1</v>
-      </c>
-      <c r="C122" s="0">
+      <c r="B122" s="1">
+        <v>1</v>
+      </c>
+      <c r="C122" s="1">
         <v>138.57289123535156</v>
       </c>
     </row>
@@ -1486,32 +1488,32 @@
       <c r="A123" t="s">
         <v>11</v>
       </c>
-      <c r="B123" s="0">
-        <v>2</v>
-      </c>
-      <c r="C123" s="0">
-        <v>145.78488159179687</v>
+      <c r="B123" s="1">
+        <v>2</v>
+      </c>
+      <c r="C123" s="1">
+        <v>145.78488159179688</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="s">
         <v>11</v>
       </c>
-      <c r="B124" s="0">
-        <v>3</v>
-      </c>
-      <c r="C124" s="0">
-        <v>168.74942016601562</v>
+      <c r="B124" s="1">
+        <v>3</v>
+      </c>
+      <c r="C124" s="1">
+        <v>168.74942016601563</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="s">
         <v>11</v>
       </c>
-      <c r="B125" s="0">
-        <v>4</v>
-      </c>
-      <c r="C125" s="0">
+      <c r="B125" s="1">
+        <v>4</v>
+      </c>
+      <c r="C125" s="1">
         <v>129.51087951660156</v>
       </c>
     </row>
@@ -1519,10 +1521,10 @@
       <c r="A126" t="s">
         <v>11</v>
       </c>
-      <c r="B126" s="0">
-        <v>5</v>
-      </c>
-      <c r="C126" s="0">
+      <c r="B126" s="1">
+        <v>5</v>
+      </c>
+      <c r="C126" s="1">
         <v>112.51808166503906</v>
       </c>
     </row>
@@ -1530,10 +1532,10 @@
       <c r="A127" t="s">
         <v>11</v>
       </c>
-      <c r="B127" s="0">
-        <v>6</v>
-      </c>
-      <c r="C127" s="0">
+      <c r="B127" s="1">
+        <v>6</v>
+      </c>
+      <c r="C127" s="1">
         <v>107.00999450683594</v>
       </c>
     </row>
@@ -1541,10 +1543,10 @@
       <c r="A128" t="s">
         <v>11</v>
       </c>
-      <c r="B128" s="0">
-        <v>7</v>
-      </c>
-      <c r="C128" s="0">
+      <c r="B128" s="1">
+        <v>7</v>
+      </c>
+      <c r="C128" s="1">
         <v>113.38642883300781</v>
       </c>
     </row>
@@ -1552,10 +1554,10 @@
       <c r="A129" t="s">
         <v>11</v>
       </c>
-      <c r="B129" s="0">
-        <v>8</v>
-      </c>
-      <c r="C129" s="0">
+      <c r="B129" s="1">
+        <v>8</v>
+      </c>
+      <c r="C129" s="1">
         <v>143.64463806152344</v>
       </c>
     </row>
@@ -1563,10 +1565,10 @@
       <c r="A130" t="s">
         <v>11</v>
       </c>
-      <c r="B130" s="0">
-        <v>9</v>
-      </c>
-      <c r="C130" s="0">
+      <c r="B130" s="1">
+        <v>9</v>
+      </c>
+      <c r="C130" s="1">
         <v>191.05964660644531</v>
       </c>
     </row>
@@ -1574,10 +1576,10 @@
       <c r="A131" t="s">
         <v>11</v>
       </c>
-      <c r="B131" s="0">
-        <v>10</v>
-      </c>
-      <c r="C131" s="0">
+      <c r="B131" s="1">
+        <v>10</v>
+      </c>
+      <c r="C131" s="1">
         <v>242.234375</v>
       </c>
     </row>
@@ -1585,21 +1587,21 @@
       <c r="A132" t="s">
         <v>11</v>
       </c>
-      <c r="B132" s="0">
-        <v>11</v>
-      </c>
-      <c r="C132" s="0">
-        <v>169.54904174804687</v>
+      <c r="B132" s="1">
+        <v>11</v>
+      </c>
+      <c r="C132" s="1">
+        <v>169.54904174804688</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="s">
         <v>11</v>
       </c>
-      <c r="B133" s="0">
-        <v>12</v>
-      </c>
-      <c r="C133" s="0">
+      <c r="B133" s="1">
+        <v>12</v>
+      </c>
+      <c r="C133" s="1">
         <v>123.49229431152344</v>
       </c>
     </row>
@@ -1607,10 +1609,10 @@
       <c r="A134" t="s">
         <v>12</v>
       </c>
-      <c r="B134" s="0">
-        <v>1</v>
-      </c>
-      <c r="C134" s="0">
+      <c r="B134" s="1">
+        <v>1</v>
+      </c>
+      <c r="C134" s="1">
         <v>129.44589233398438</v>
       </c>
     </row>
@@ -1618,21 +1620,21 @@
       <c r="A135" t="s">
         <v>12</v>
       </c>
-      <c r="B135" s="0">
-        <v>2</v>
-      </c>
-      <c r="C135" s="0">
-        <v>129.95285034179687</v>
+      <c r="B135" s="1">
+        <v>2</v>
+      </c>
+      <c r="C135" s="1">
+        <v>129.95285034179688</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="s">
         <v>12</v>
       </c>
-      <c r="B136" s="0">
-        <v>3</v>
-      </c>
-      <c r="C136" s="0">
+      <c r="B136" s="1">
+        <v>3</v>
+      </c>
+      <c r="C136" s="1">
         <v>111.89681243896484</v>
       </c>
     </row>
@@ -1640,10 +1642,10 @@
       <c r="A137" t="s">
         <v>12</v>
       </c>
-      <c r="B137" s="0">
-        <v>4</v>
-      </c>
-      <c r="C137" s="0">
+      <c r="B137" s="1">
+        <v>4</v>
+      </c>
+      <c r="C137" s="1">
         <v>111.6890869140625</v>
       </c>
     </row>
@@ -1651,10 +1653,10 @@
       <c r="A138" t="s">
         <v>12</v>
       </c>
-      <c r="B138" s="0">
-        <v>5</v>
-      </c>
-      <c r="C138" s="0">
+      <c r="B138" s="1">
+        <v>5</v>
+      </c>
+      <c r="C138" s="1">
         <v>116.61088562011719</v>
       </c>
     </row>
@@ -1662,21 +1664,21 @@
       <c r="A139" t="s">
         <v>12</v>
       </c>
-      <c r="B139" s="0">
-        <v>6</v>
-      </c>
-      <c r="C139" s="0">
-        <v>154.18637084960937</v>
+      <c r="B139" s="1">
+        <v>6</v>
+      </c>
+      <c r="C139" s="1">
+        <v>154.18637084960938</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="s">
         <v>12</v>
       </c>
-      <c r="B140" s="0">
-        <v>7</v>
-      </c>
-      <c r="C140" s="0">
+      <c r="B140" s="1">
+        <v>7</v>
+      </c>
+      <c r="C140" s="1">
         <v>128.96145629882813</v>
       </c>
     </row>
@@ -1684,21 +1686,21 @@
       <c r="A141" t="s">
         <v>12</v>
       </c>
-      <c r="B141" s="0">
-        <v>8</v>
-      </c>
-      <c r="C141" s="0">
-        <v>117.74832153320312</v>
+      <c r="B141" s="1">
+        <v>8</v>
+      </c>
+      <c r="C141" s="1">
+        <v>117.74832153320313</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="s">
         <v>12</v>
       </c>
-      <c r="B142" s="0">
-        <v>9</v>
-      </c>
-      <c r="C142" s="0">
+      <c r="B142" s="1">
+        <v>9</v>
+      </c>
+      <c r="C142" s="1">
         <v>100.07635498046875</v>
       </c>
     </row>
@@ -1706,10 +1708,10 @@
       <c r="A143" t="s">
         <v>12</v>
       </c>
-      <c r="B143" s="0">
-        <v>10</v>
-      </c>
-      <c r="C143" s="0">
+      <c r="B143" s="1">
+        <v>10</v>
+      </c>
+      <c r="C143" s="1">
         <v>107.54240417480469</v>
       </c>
     </row>
@@ -1717,10 +1719,10 @@
       <c r="A144" t="s">
         <v>12</v>
       </c>
-      <c r="B144" s="0">
-        <v>11</v>
-      </c>
-      <c r="C144" s="0">
+      <c r="B144" s="1">
+        <v>11</v>
+      </c>
+      <c r="C144" s="1">
         <v>107.57199859619141</v>
       </c>
     </row>
@@ -1728,10 +1730,10 @@
       <c r="A145" t="s">
         <v>12</v>
       </c>
-      <c r="B145" s="0">
-        <v>12</v>
-      </c>
-      <c r="C145" s="0">
+      <c r="B145" s="1">
+        <v>12</v>
+      </c>
+      <c r="C145" s="1">
         <v>135.97782897949219</v>
       </c>
     </row>
@@ -1739,10 +1741,10 @@
       <c r="A146" t="s">
         <v>13</v>
       </c>
-      <c r="B146" s="0">
-        <v>1</v>
-      </c>
-      <c r="C146" s="0">
+      <c r="B146" s="1">
+        <v>1</v>
+      </c>
+      <c r="C146" s="1">
         <v>148.26554870605469</v>
       </c>
     </row>
@@ -1750,10 +1752,10 @@
       <c r="A147" t="s">
         <v>13</v>
       </c>
-      <c r="B147" s="0">
-        <v>2</v>
-      </c>
-      <c r="C147" s="0">
+      <c r="B147" s="1">
+        <v>2</v>
+      </c>
+      <c r="C147" s="1">
         <v>143.34239196777344</v>
       </c>
     </row>
@@ -1761,10 +1763,10 @@
       <c r="A148" t="s">
         <v>13</v>
       </c>
-      <c r="B148" s="0">
-        <v>3</v>
-      </c>
-      <c r="C148" s="0">
+      <c r="B148" s="1">
+        <v>3</v>
+      </c>
+      <c r="C148" s="1">
         <v>160.08869934082031</v>
       </c>
     </row>
@@ -1772,10 +1774,10 @@
       <c r="A149" t="s">
         <v>13</v>
       </c>
-      <c r="B149" s="0">
-        <v>4</v>
-      </c>
-      <c r="C149" s="0">
+      <c r="B149" s="1">
+        <v>4</v>
+      </c>
+      <c r="C149" s="1">
         <v>161.00445556640625</v>
       </c>
     </row>
@@ -1783,10 +1785,10 @@
       <c r="A150" t="s">
         <v>13</v>
       </c>
-      <c r="B150" s="0">
-        <v>5</v>
-      </c>
-      <c r="C150" s="0">
+      <c r="B150" s="1">
+        <v>5</v>
+      </c>
+      <c r="C150" s="1">
         <v>243.53857421875</v>
       </c>
     </row>
@@ -1794,21 +1796,21 @@
       <c r="A151" t="s">
         <v>13</v>
       </c>
-      <c r="B151" s="0">
-        <v>6</v>
-      </c>
-      <c r="C151" s="0">
-        <v>184.01828002929687</v>
+      <c r="B151" s="1">
+        <v>6</v>
+      </c>
+      <c r="C151" s="1">
+        <v>184.01828002929688</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="s">
         <v>13</v>
       </c>
-      <c r="B152" s="0">
-        <v>7</v>
-      </c>
-      <c r="C152" s="0">
+      <c r="B152" s="1">
+        <v>7</v>
+      </c>
+      <c r="C152" s="1">
         <v>142.86163330078125</v>
       </c>
     </row>
@@ -1816,21 +1818,21 @@
       <c r="A153" t="s">
         <v>13</v>
       </c>
-      <c r="B153" s="0">
-        <v>8</v>
-      </c>
-      <c r="C153" s="0">
-        <v>165.98422241210937</v>
+      <c r="B153" s="1">
+        <v>8</v>
+      </c>
+      <c r="C153" s="1">
+        <v>165.98422241210938</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="s">
         <v>13</v>
       </c>
-      <c r="B154" s="0">
-        <v>9</v>
-      </c>
-      <c r="C154" s="0">
+      <c r="B154" s="1">
+        <v>9</v>
+      </c>
+      <c r="C154" s="1">
         <v>127.90261840820313</v>
       </c>
     </row>
@@ -1838,10 +1840,10 @@
       <c r="A155" t="s">
         <v>13</v>
       </c>
-      <c r="B155" s="0">
-        <v>10</v>
-      </c>
-      <c r="C155" s="0">
+      <c r="B155" s="1">
+        <v>10</v>
+      </c>
+      <c r="C155" s="1">
         <v>177.80287170410156</v>
       </c>
     </row>
@@ -1849,10 +1851,10 @@
       <c r="A156" t="s">
         <v>13</v>
       </c>
-      <c r="B156" s="0">
-        <v>11</v>
-      </c>
-      <c r="C156" s="0">
+      <c r="B156" s="1">
+        <v>11</v>
+      </c>
+      <c r="C156" s="1">
         <v>153.24842834472656</v>
       </c>
     </row>
@@ -1860,10 +1862,10 @@
       <c r="A157" t="s">
         <v>13</v>
       </c>
-      <c r="B157" s="0">
-        <v>12</v>
-      </c>
-      <c r="C157" s="0">
+      <c r="B157" s="1">
+        <v>12</v>
+      </c>
+      <c r="C157" s="1">
         <v>122.77899169921875</v>
       </c>
     </row>
@@ -1871,21 +1873,21 @@
       <c r="A158" t="s">
         <v>14</v>
       </c>
-      <c r="B158" s="0">
-        <v>1</v>
-      </c>
-      <c r="C158" s="0">
-        <v>123.68014526367187</v>
+      <c r="B158" s="1">
+        <v>1</v>
+      </c>
+      <c r="C158" s="1">
+        <v>123.68014526367188</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="s">
         <v>14</v>
       </c>
-      <c r="B159" s="0">
-        <v>2</v>
-      </c>
-      <c r="C159" s="0">
+      <c r="B159" s="1">
+        <v>2</v>
+      </c>
+      <c r="C159" s="1">
         <v>119.12128448486328</v>
       </c>
     </row>
@@ -1893,10 +1895,10 @@
       <c r="A160" t="s">
         <v>14</v>
       </c>
-      <c r="B160" s="0">
-        <v>3</v>
-      </c>
-      <c r="C160" s="0">
+      <c r="B160" s="1">
+        <v>3</v>
+      </c>
+      <c r="C160" s="1">
         <v>131.42254638671875</v>
       </c>
     </row>
@@ -1904,10 +1906,10 @@
       <c r="A161" t="s">
         <v>14</v>
       </c>
-      <c r="B161" s="0">
-        <v>4</v>
-      </c>
-      <c r="C161" s="0">
+      <c r="B161" s="1">
+        <v>4</v>
+      </c>
+      <c r="C161" s="1">
         <v>97.936988830566406</v>
       </c>
     </row>
@@ -1915,10 +1917,10 @@
       <c r="A162" t="s">
         <v>14</v>
       </c>
-      <c r="B162" s="0">
-        <v>5</v>
-      </c>
-      <c r="C162" s="0">
+      <c r="B162" s="1">
+        <v>5</v>
+      </c>
+      <c r="C162" s="1">
         <v>94.244071960449219</v>
       </c>
     </row>
@@ -1926,10 +1928,10 @@
       <c r="A163" t="s">
         <v>14</v>
       </c>
-      <c r="B163" s="0">
-        <v>6</v>
-      </c>
-      <c r="C163" s="0">
+      <c r="B163" s="1">
+        <v>6</v>
+      </c>
+      <c r="C163" s="1">
         <v>122.69766998291016</v>
       </c>
     </row>
@@ -1937,21 +1939,21 @@
       <c r="A164" t="s">
         <v>14</v>
       </c>
-      <c r="B164" s="0">
-        <v>7</v>
-      </c>
-      <c r="C164" s="0">
-        <v>149.02828979492187</v>
+      <c r="B164" s="1">
+        <v>7</v>
+      </c>
+      <c r="C164" s="1">
+        <v>149.02828979492188</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="s">
         <v>14</v>
       </c>
-      <c r="B165" s="0">
-        <v>8</v>
-      </c>
-      <c r="C165" s="0">
+      <c r="B165" s="1">
+        <v>8</v>
+      </c>
+      <c r="C165" s="1">
         <v>177.75312805175781</v>
       </c>
     </row>
@@ -1959,10 +1961,10 @@
       <c r="A166" t="s">
         <v>14</v>
       </c>
-      <c r="B166" s="0">
-        <v>9</v>
-      </c>
-      <c r="C166" s="0">
+      <c r="B166" s="1">
+        <v>9</v>
+      </c>
+      <c r="C166" s="1">
         <v>153.32763671875</v>
       </c>
     </row>
@@ -1970,10 +1972,10 @@
       <c r="A167" t="s">
         <v>14</v>
       </c>
-      <c r="B167" s="0">
-        <v>10</v>
-      </c>
-      <c r="C167" s="0">
+      <c r="B167" s="1">
+        <v>10</v>
+      </c>
+      <c r="C167" s="1">
         <v>149.69090270996094</v>
       </c>
     </row>
@@ -1981,10 +1983,10 @@
       <c r="A168" t="s">
         <v>14</v>
       </c>
-      <c r="B168" s="0">
-        <v>11</v>
-      </c>
-      <c r="C168" s="0">
+      <c r="B168" s="1">
+        <v>11</v>
+      </c>
+      <c r="C168" s="1">
         <v>209.89849853515625</v>
       </c>
     </row>
@@ -1992,10 +1994,10 @@
       <c r="A169" t="s">
         <v>14</v>
       </c>
-      <c r="B169" s="0">
-        <v>12</v>
-      </c>
-      <c r="C169" s="0">
+      <c r="B169" s="1">
+        <v>12</v>
+      </c>
+      <c r="C169" s="1">
         <v>140.62797546386719</v>
       </c>
     </row>
@@ -2003,10 +2005,10 @@
       <c r="A170" t="s">
         <v>15</v>
       </c>
-      <c r="B170" s="0">
-        <v>1</v>
-      </c>
-      <c r="C170" s="0">
+      <c r="B170" s="1">
+        <v>1</v>
+      </c>
+      <c r="C170" s="1">
         <v>137.26155090332031</v>
       </c>
     </row>
@@ -2014,10 +2016,10 @@
       <c r="A171" t="s">
         <v>15</v>
       </c>
-      <c r="B171" s="0">
-        <v>2</v>
-      </c>
-      <c r="C171" s="0">
+      <c r="B171" s="1">
+        <v>2</v>
+      </c>
+      <c r="C171" s="1">
         <v>132.02021789550781</v>
       </c>
     </row>
@@ -2025,10 +2027,10 @@
       <c r="A172" t="s">
         <v>15</v>
       </c>
-      <c r="B172" s="0">
-        <v>3</v>
-      </c>
-      <c r="C172" s="0">
+      <c r="B172" s="1">
+        <v>3</v>
+      </c>
+      <c r="C172" s="1">
         <v>103.72963714599609</v>
       </c>
     </row>
@@ -2036,10 +2038,10 @@
       <c r="A173" t="s">
         <v>15</v>
       </c>
-      <c r="B173" s="0">
-        <v>4</v>
-      </c>
-      <c r="C173" s="0">
+      <c r="B173" s="1">
+        <v>4</v>
+      </c>
+      <c r="C173" s="1">
         <v>109.31269073486328</v>
       </c>
     </row>
@@ -2047,10 +2049,10 @@
       <c r="A174" t="s">
         <v>15</v>
       </c>
-      <c r="B174" s="0">
-        <v>5</v>
-      </c>
-      <c r="C174" s="0">
+      <c r="B174" s="1">
+        <v>5</v>
+      </c>
+      <c r="C174" s="1">
         <v>151.78517150878906</v>
       </c>
     </row>
@@ -2058,10 +2060,10 @@
       <c r="A175" t="s">
         <v>15</v>
       </c>
-      <c r="B175" s="0">
-        <v>6</v>
-      </c>
-      <c r="C175" s="0">
+      <c r="B175" s="1">
+        <v>6</v>
+      </c>
+      <c r="C175" s="1">
         <v>169.64906311035156</v>
       </c>
     </row>
@@ -2069,10 +2071,10 @@
       <c r="A176" t="s">
         <v>15</v>
       </c>
-      <c r="B176" s="0">
-        <v>7</v>
-      </c>
-      <c r="C176" s="0">
+      <c r="B176" s="1">
+        <v>7</v>
+      </c>
+      <c r="C176" s="1">
         <v>129.98323059082031</v>
       </c>
     </row>
@@ -2080,10 +2082,10 @@
       <c r="A177" t="s">
         <v>15</v>
       </c>
-      <c r="B177" s="0">
-        <v>8</v>
-      </c>
-      <c r="C177" s="0">
+      <c r="B177" s="1">
+        <v>8</v>
+      </c>
+      <c r="C177" s="1">
         <v>98.178688049316406</v>
       </c>
     </row>
@@ -2091,10 +2093,10 @@
       <c r="A178" t="s">
         <v>15</v>
       </c>
-      <c r="B178" s="0">
-        <v>9</v>
-      </c>
-      <c r="C178" s="0">
+      <c r="B178" s="1">
+        <v>9</v>
+      </c>
+      <c r="C178" s="1">
         <v>124.43543243408203</v>
       </c>
     </row>
@@ -2102,21 +2104,21 @@
       <c r="A179" t="s">
         <v>15</v>
       </c>
-      <c r="B179" s="0">
-        <v>10</v>
-      </c>
-      <c r="C179" s="0">
-        <v>153.99227905273437</v>
+      <c r="B179" s="1">
+        <v>10</v>
+      </c>
+      <c r="C179" s="1">
+        <v>153.99227905273438</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="s">
         <v>15</v>
       </c>
-      <c r="B180" s="0">
-        <v>11</v>
-      </c>
-      <c r="C180" s="0">
+      <c r="B180" s="1">
+        <v>11</v>
+      </c>
+      <c r="C180" s="1">
         <v>162.10096740722656</v>
       </c>
     </row>
@@ -2124,10 +2126,10 @@
       <c r="A181" t="s">
         <v>15</v>
       </c>
-      <c r="B181" s="0">
-        <v>12</v>
-      </c>
-      <c r="C181" s="0">
+      <c r="B181" s="1">
+        <v>12</v>
+      </c>
+      <c r="C181" s="1">
         <v>140.64390563964844</v>
       </c>
     </row>
@@ -2135,21 +2137,21 @@
       <c r="A182" t="s">
         <v>16</v>
       </c>
-      <c r="B182" s="0">
-        <v>1</v>
-      </c>
-      <c r="C182" s="0">
-        <v>187.77023315429687</v>
+      <c r="B182" s="1">
+        <v>1</v>
+      </c>
+      <c r="C182" s="1">
+        <v>187.77023315429688</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="s">
         <v>16</v>
       </c>
-      <c r="B183" s="0">
-        <v>2</v>
-      </c>
-      <c r="C183" s="0">
+      <c r="B183" s="1">
+        <v>2</v>
+      </c>
+      <c r="C183" s="1">
         <v>97.381301879882813</v>
       </c>
     </row>
@@ -2157,21 +2159,21 @@
       <c r="A184" t="s">
         <v>16</v>
       </c>
-      <c r="B184" s="0">
-        <v>3</v>
-      </c>
-      <c r="C184" s="0">
-        <v>108.96334838867187</v>
+      <c r="B184" s="1">
+        <v>3</v>
+      </c>
+      <c r="C184" s="1">
+        <v>108.96334838867188</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="s">
         <v>16</v>
       </c>
-      <c r="B185" s="0">
-        <v>4</v>
-      </c>
-      <c r="C185" s="0">
+      <c r="B185" s="1">
+        <v>4</v>
+      </c>
+      <c r="C185" s="1">
         <v>101.40814971923828</v>
       </c>
     </row>
@@ -2179,10 +2181,10 @@
       <c r="A186" t="s">
         <v>16</v>
       </c>
-      <c r="B186" s="0">
-        <v>5</v>
-      </c>
-      <c r="C186" s="0">
+      <c r="B186" s="1">
+        <v>5</v>
+      </c>
+      <c r="C186" s="1">
         <v>72.982437133789063</v>
       </c>
     </row>
@@ -2190,10 +2192,10 @@
       <c r="A187" t="s">
         <v>16</v>
       </c>
-      <c r="B187" s="0">
-        <v>6</v>
-      </c>
-      <c r="C187" s="0">
+      <c r="B187" s="1">
+        <v>6</v>
+      </c>
+      <c r="C187" s="1">
         <v>90.508140563964844</v>
       </c>
     </row>
@@ -2201,10 +2203,10 @@
       <c r="A188" t="s">
         <v>16</v>
       </c>
-      <c r="B188" s="0">
-        <v>7</v>
-      </c>
-      <c r="C188" s="0">
+      <c r="B188" s="1">
+        <v>7</v>
+      </c>
+      <c r="C188" s="1">
         <v>68.187995910644531</v>
       </c>
     </row>
@@ -2212,10 +2214,10 @@
       <c r="A189" t="s">
         <v>16</v>
       </c>
-      <c r="B189" s="0">
-        <v>8</v>
-      </c>
-      <c r="C189" s="0">
+      <c r="B189" s="1">
+        <v>8</v>
+      </c>
+      <c r="C189" s="1">
         <v>91.647727966308594</v>
       </c>
     </row>
@@ -2223,10 +2225,10 @@
       <c r="A190" t="s">
         <v>16</v>
       </c>
-      <c r="B190" s="0">
-        <v>9</v>
-      </c>
-      <c r="C190" s="0">
+      <c r="B190" s="1">
+        <v>9</v>
+      </c>
+      <c r="C190" s="1">
         <v>94.262176513671875</v>
       </c>
     </row>
@@ -2234,10 +2236,10 @@
       <c r="A191" t="s">
         <v>16</v>
       </c>
-      <c r="B191" s="0">
-        <v>10</v>
-      </c>
-      <c r="C191" s="0">
+      <c r="B191" s="1">
+        <v>10</v>
+      </c>
+      <c r="C191" s="1">
         <v>110.99637603759766</v>
       </c>
     </row>
@@ -2245,10 +2247,10 @@
       <c r="A192" t="s">
         <v>16</v>
       </c>
-      <c r="B192" s="0">
-        <v>11</v>
-      </c>
-      <c r="C192" s="0">
+      <c r="B192" s="1">
+        <v>11</v>
+      </c>
+      <c r="C192" s="1">
         <v>82.074790954589844</v>
       </c>
     </row>
@@ -2256,10 +2258,10 @@
       <c r="A193" t="s">
         <v>16</v>
       </c>
-      <c r="B193" s="0">
-        <v>12</v>
-      </c>
-      <c r="C193" s="0">
+      <c r="B193" s="1">
+        <v>12</v>
+      </c>
+      <c r="C193" s="1">
         <v>89.423934936523438</v>
       </c>
     </row>
@@ -2267,10 +2269,10 @@
       <c r="A194" t="s">
         <v>17</v>
       </c>
-      <c r="B194" s="0">
-        <v>1</v>
-      </c>
-      <c r="C194" s="0">
+      <c r="B194" s="1">
+        <v>1</v>
+      </c>
+      <c r="C194" s="1">
         <v>103.99873352050781</v>
       </c>
     </row>
@@ -2278,10 +2280,10 @@
       <c r="A195" t="s">
         <v>17</v>
       </c>
-      <c r="B195" s="0">
-        <v>2</v>
-      </c>
-      <c r="C195" s="0">
+      <c r="B195" s="1">
+        <v>2</v>
+      </c>
+      <c r="C195" s="1">
         <v>117.69552612304688</v>
       </c>
     </row>
@@ -2289,10 +2291,10 @@
       <c r="A196" t="s">
         <v>17</v>
       </c>
-      <c r="B196" s="0">
-        <v>3</v>
-      </c>
-      <c r="C196" s="0">
+      <c r="B196" s="1">
+        <v>3</v>
+      </c>
+      <c r="C196" s="1">
         <v>111.04788970947266</v>
       </c>
     </row>
@@ -2300,10 +2302,10 @@
       <c r="A197" t="s">
         <v>17</v>
       </c>
-      <c r="B197" s="0">
-        <v>4</v>
-      </c>
-      <c r="C197" s="0">
+      <c r="B197" s="1">
+        <v>4</v>
+      </c>
+      <c r="C197" s="1">
         <v>71.126228332519531</v>
       </c>
     </row>
@@ -2311,10 +2313,10 @@
       <c r="A198" t="s">
         <v>17</v>
       </c>
-      <c r="B198" s="0">
-        <v>5</v>
-      </c>
-      <c r="C198" s="0">
+      <c r="B198" s="1">
+        <v>5</v>
+      </c>
+      <c r="C198" s="1">
         <v>90.164924621582031</v>
       </c>
     </row>
@@ -2322,10 +2324,10 @@
       <c r="A199" t="s">
         <v>17</v>
       </c>
-      <c r="B199" s="0">
-        <v>6</v>
-      </c>
-      <c r="C199" s="0">
+      <c r="B199" s="1">
+        <v>6</v>
+      </c>
+      <c r="C199" s="1">
         <v>68.777374267578125</v>
       </c>
     </row>
@@ -2333,10 +2335,10 @@
       <c r="A200" t="s">
         <v>17</v>
       </c>
-      <c r="B200" s="0">
-        <v>7</v>
-      </c>
-      <c r="C200" s="0">
+      <c r="B200" s="1">
+        <v>7</v>
+      </c>
+      <c r="C200" s="1">
         <v>62.335445404052734</v>
       </c>
     </row>
@@ -2344,10 +2346,10 @@
       <c r="A201" t="s">
         <v>17</v>
       </c>
-      <c r="B201" s="0">
-        <v>8</v>
-      </c>
-      <c r="C201" s="0">
+      <c r="B201" s="1">
+        <v>8</v>
+      </c>
+      <c r="C201" s="1">
         <v>132.47334289550781</v>
       </c>
     </row>
@@ -2355,21 +2357,21 @@
       <c r="A202" t="s">
         <v>17</v>
       </c>
-      <c r="B202" s="0">
-        <v>9</v>
-      </c>
-      <c r="C202" s="0">
-        <v>176.28372192382812</v>
+      <c r="B202" s="1">
+        <v>9</v>
+      </c>
+      <c r="C202" s="1">
+        <v>176.28372192382813</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="s">
         <v>17</v>
       </c>
-      <c r="B203" s="0">
-        <v>10</v>
-      </c>
-      <c r="C203" s="0">
+      <c r="B203" s="1">
+        <v>10</v>
+      </c>
+      <c r="C203" s="1">
         <v>95.969215393066406</v>
       </c>
     </row>
@@ -2377,10 +2379,10 @@
       <c r="A204" t="s">
         <v>17</v>
       </c>
-      <c r="B204" s="0">
-        <v>11</v>
-      </c>
-      <c r="C204" s="0">
+      <c r="B204" s="1">
+        <v>11</v>
+      </c>
+      <c r="C204" s="1">
         <v>86.566505432128906</v>
       </c>
     </row>
@@ -2388,32 +2390,32 @@
       <c r="A205" t="s">
         <v>17</v>
       </c>
-      <c r="B205" s="0">
-        <v>12</v>
-      </c>
-      <c r="C205" s="0">
-        <v>121.59109497070312</v>
+      <c r="B205" s="1">
+        <v>12</v>
+      </c>
+      <c r="C205" s="1">
+        <v>121.59109497070313</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="s">
         <v>18</v>
       </c>
-      <c r="B206" s="0">
-        <v>1</v>
-      </c>
-      <c r="C206" s="0">
-        <v>135.73043823242187</v>
+      <c r="B206" s="1">
+        <v>1</v>
+      </c>
+      <c r="C206" s="1">
+        <v>135.73043823242188</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="s">
         <v>18</v>
       </c>
-      <c r="B207" s="0">
-        <v>2</v>
-      </c>
-      <c r="C207" s="0">
+      <c r="B207" s="1">
+        <v>2</v>
+      </c>
+      <c r="C207" s="1">
         <v>119.0836181640625</v>
       </c>
     </row>
@@ -2421,10 +2423,10 @@
       <c r="A208" t="s">
         <v>18</v>
       </c>
-      <c r="B208" s="0">
-        <v>3</v>
-      </c>
-      <c r="C208" s="0">
+      <c r="B208" s="1">
+        <v>3</v>
+      </c>
+      <c r="C208" s="1">
         <v>131.49864196777344</v>
       </c>
     </row>
@@ -2432,10 +2434,10 @@
       <c r="A209" t="s">
         <v>18</v>
       </c>
-      <c r="B209" s="0">
-        <v>4</v>
-      </c>
-      <c r="C209" s="0">
+      <c r="B209" s="1">
+        <v>4</v>
+      </c>
+      <c r="C209" s="1">
         <v>170.47334289550781</v>
       </c>
     </row>
@@ -2443,10 +2445,10 @@
       <c r="A210" t="s">
         <v>18</v>
       </c>
-      <c r="B210" s="0">
-        <v>5</v>
-      </c>
-      <c r="C210" s="0">
+      <c r="B210" s="1">
+        <v>5</v>
+      </c>
+      <c r="C210" s="1">
         <v>140.91246032714844</v>
       </c>
     </row>
@@ -2454,10 +2456,10 @@
       <c r="A211" t="s">
         <v>18</v>
       </c>
-      <c r="B211" s="0">
-        <v>6</v>
-      </c>
-      <c r="C211" s="0">
+      <c r="B211" s="1">
+        <v>6</v>
+      </c>
+      <c r="C211" s="1">
         <v>148.81655883789063</v>
       </c>
     </row>
@@ -2465,10 +2467,10 @@
       <c r="A212" t="s">
         <v>18</v>
       </c>
-      <c r="B212" s="0">
-        <v>7</v>
-      </c>
-      <c r="C212" s="0">
+      <c r="B212" s="1">
+        <v>7</v>
+      </c>
+      <c r="C212" s="1">
         <v>136.10011291503906</v>
       </c>
     </row>
@@ -2476,10 +2478,10 @@
       <c r="A213" t="s">
         <v>18</v>
       </c>
-      <c r="B213" s="0">
-        <v>8</v>
-      </c>
-      <c r="C213" s="0">
+      <c r="B213" s="1">
+        <v>8</v>
+      </c>
+      <c r="C213" s="1">
         <v>86.1436767578125</v>
       </c>
     </row>
@@ -2487,10 +2489,10 @@
       <c r="A214" t="s">
         <v>18</v>
       </c>
-      <c r="B214" s="0">
-        <v>9</v>
-      </c>
-      <c r="C214" s="0">
+      <c r="B214" s="1">
+        <v>9</v>
+      </c>
+      <c r="C214" s="1">
         <v>135.07499694824219</v>
       </c>
     </row>
@@ -2498,10 +2500,10 @@
       <c r="A215" t="s">
         <v>18</v>
       </c>
-      <c r="B215" s="0">
-        <v>10</v>
-      </c>
-      <c r="C215" s="0">
+      <c r="B215" s="1">
+        <v>10</v>
+      </c>
+      <c r="C215" s="1">
         <v>89.914527893066406</v>
       </c>
     </row>
@@ -2509,10 +2511,10 @@
       <c r="A216" t="s">
         <v>18</v>
       </c>
-      <c r="B216" s="0">
-        <v>11</v>
-      </c>
-      <c r="C216" s="0">
+      <c r="B216" s="1">
+        <v>11</v>
+      </c>
+      <c r="C216" s="1">
         <v>120.86214447021484</v>
       </c>
     </row>
@@ -2520,21 +2522,21 @@
       <c r="A217" t="s">
         <v>18</v>
       </c>
-      <c r="B217" s="0">
-        <v>12</v>
-      </c>
-      <c r="C217" s="0">
-        <v>82.872787475585937</v>
+      <c r="B217" s="1">
+        <v>12</v>
+      </c>
+      <c r="C217" s="1">
+        <v>82.872787475585938</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="s">
         <v>19</v>
       </c>
-      <c r="B218" s="0">
-        <v>1</v>
-      </c>
-      <c r="C218" s="0">
+      <c r="B218" s="1">
+        <v>1</v>
+      </c>
+      <c r="C218" s="1">
         <v>135.63230895996094</v>
       </c>
     </row>
@@ -2542,10 +2544,10 @@
       <c r="A219" t="s">
         <v>19</v>
       </c>
-      <c r="B219" s="0">
-        <v>2</v>
-      </c>
-      <c r="C219" s="0">
+      <c r="B219" s="1">
+        <v>2</v>
+      </c>
+      <c r="C219" s="1">
         <v>190.81669616699219</v>
       </c>
     </row>
@@ -2553,10 +2555,10 @@
       <c r="A220" t="s">
         <v>19</v>
       </c>
-      <c r="B220" s="0">
-        <v>3</v>
-      </c>
-      <c r="C220" s="0">
+      <c r="B220" s="1">
+        <v>3</v>
+      </c>
+      <c r="C220" s="1">
         <v>290.92950439453125</v>
       </c>
     </row>
@@ -2564,10 +2566,10 @@
       <c r="A221" t="s">
         <v>19</v>
       </c>
-      <c r="B221" s="0">
-        <v>4</v>
-      </c>
-      <c r="C221" s="0">
+      <c r="B221" s="1">
+        <v>4</v>
+      </c>
+      <c r="C221" s="1">
         <v>197.17079162597656</v>
       </c>
     </row>
@@ -2575,32 +2577,32 @@
       <c r="A222" t="s">
         <v>19</v>
       </c>
-      <c r="B222" s="0">
-        <v>5</v>
-      </c>
-      <c r="C222" s="0">
-        <v>246.75491333007812</v>
+      <c r="B222" s="1">
+        <v>5</v>
+      </c>
+      <c r="C222" s="1">
+        <v>246.75491333007813</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="s">
         <v>19</v>
       </c>
-      <c r="B223" s="0">
-        <v>6</v>
-      </c>
-      <c r="C223" s="0">
-        <v>503.94247436523437</v>
+      <c r="B223" s="1">
+        <v>6</v>
+      </c>
+      <c r="C223" s="1">
+        <v>503.94247436523438</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="s">
         <v>19</v>
       </c>
-      <c r="B224" s="0">
-        <v>7</v>
-      </c>
-      <c r="C224" s="0">
+      <c r="B224" s="1">
+        <v>7</v>
+      </c>
+      <c r="C224" s="1">
         <v>558.2236328125</v>
       </c>
     </row>
@@ -2608,21 +2610,21 @@
       <c r="A225" t="s">
         <v>19</v>
       </c>
-      <c r="B225" s="0">
-        <v>8</v>
-      </c>
-      <c r="C225" s="0">
-        <v>311.36483764648437</v>
+      <c r="B225" s="1">
+        <v>8</v>
+      </c>
+      <c r="C225" s="1">
+        <v>311.36483764648438</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="s">
         <v>19</v>
       </c>
-      <c r="B226" s="0">
-        <v>9</v>
-      </c>
-      <c r="C226" s="0">
+      <c r="B226" s="1">
+        <v>9</v>
+      </c>
+      <c r="C226" s="1">
         <v>209.637939453125</v>
       </c>
     </row>
@@ -2630,10 +2632,10 @@
       <c r="A227" t="s">
         <v>19</v>
       </c>
-      <c r="B227" s="0">
-        <v>10</v>
-      </c>
-      <c r="C227" s="0">
+      <c r="B227" s="1">
+        <v>10</v>
+      </c>
+      <c r="C227" s="1">
         <v>270.02349853515625</v>
       </c>
     </row>
@@ -2641,21 +2643,21 @@
       <c r="A228" t="s">
         <v>19</v>
       </c>
-      <c r="B228" s="0">
-        <v>11</v>
-      </c>
-      <c r="C228" s="0">
-        <v>358.82839965820312</v>
+      <c r="B228" s="1">
+        <v>11</v>
+      </c>
+      <c r="C228" s="1">
+        <v>358.82839965820313</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="s">
         <v>19</v>
       </c>
-      <c r="B229" s="0">
-        <v>12</v>
-      </c>
-      <c r="C229" s="0">
+      <c r="B229" s="1">
+        <v>12</v>
+      </c>
+      <c r="C229" s="1">
         <v>196.34368896484375</v>
       </c>
     </row>
@@ -2663,10 +2665,10 @@
       <c r="A230" t="s">
         <v>20</v>
       </c>
-      <c r="B230" s="0">
-        <v>1</v>
-      </c>
-      <c r="C230" s="0">
+      <c r="B230" s="1">
+        <v>1</v>
+      </c>
+      <c r="C230" s="1">
         <v>257.848388671875</v>
       </c>
     </row>
@@ -2674,21 +2676,21 @@
       <c r="A231" t="s">
         <v>20</v>
       </c>
-      <c r="B231" s="0">
-        <v>2</v>
-      </c>
-      <c r="C231" s="0">
-        <v>194.04470825195312</v>
+      <c r="B231" s="1">
+        <v>2</v>
+      </c>
+      <c r="C231" s="1">
+        <v>194.04470825195313</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="s">
         <v>20</v>
       </c>
-      <c r="B232" s="0">
-        <v>3</v>
-      </c>
-      <c r="C232" s="0">
+      <c r="B232" s="1">
+        <v>3</v>
+      </c>
+      <c r="C232" s="1">
         <v>232.45973205566406</v>
       </c>
     </row>
@@ -2696,10 +2698,10 @@
       <c r="A233" t="s">
         <v>20</v>
       </c>
-      <c r="B233" s="0">
-        <v>4</v>
-      </c>
-      <c r="C233" s="0">
+      <c r="B233" s="1">
+        <v>4</v>
+      </c>
+      <c r="C233" s="1">
         <v>169.176025390625</v>
       </c>
     </row>
@@ -2707,10 +2709,10 @@
       <c r="A234" t="s">
         <v>20</v>
       </c>
-      <c r="B234" s="0">
-        <v>5</v>
-      </c>
-      <c r="C234" s="0">
+      <c r="B234" s="1">
+        <v>5</v>
+      </c>
+      <c r="C234" s="1">
         <v>159.40144348144531</v>
       </c>
     </row>
@@ -2718,10 +2720,10 @@
       <c r="A235" t="s">
         <v>20</v>
       </c>
-      <c r="B235" s="0">
-        <v>6</v>
-      </c>
-      <c r="C235" s="0">
+      <c r="B235" s="1">
+        <v>6</v>
+      </c>
+      <c r="C235" s="1">
         <v>318.99114990234375</v>
       </c>
     </row>
@@ -2729,10 +2731,10 @@
       <c r="A236" t="s">
         <v>20</v>
       </c>
-      <c r="B236" s="0">
-        <v>7</v>
-      </c>
-      <c r="C236" s="0">
+      <c r="B236" s="1">
+        <v>7</v>
+      </c>
+      <c r="C236" s="1">
         <v>183.65895080566406</v>
       </c>
     </row>
@@ -2740,10 +2742,10 @@
       <c r="A237" t="s">
         <v>20</v>
       </c>
-      <c r="B237" s="0">
-        <v>8</v>
-      </c>
-      <c r="C237" s="0">
+      <c r="B237" s="1">
+        <v>8</v>
+      </c>
+      <c r="C237" s="1">
         <v>151.20429992675781</v>
       </c>
     </row>
@@ -2751,10 +2753,10 @@
       <c r="A238" t="s">
         <v>20</v>
       </c>
-      <c r="B238" s="0">
-        <v>9</v>
-      </c>
-      <c r="C238" s="0">
+      <c r="B238" s="1">
+        <v>9</v>
+      </c>
+      <c r="C238" s="1">
         <v>140.77882385253906</v>
       </c>
     </row>
@@ -2762,10 +2764,10 @@
       <c r="A239" t="s">
         <v>20</v>
       </c>
-      <c r="B239" s="0">
-        <v>10</v>
-      </c>
-      <c r="C239" s="0">
+      <c r="B239" s="1">
+        <v>10</v>
+      </c>
+      <c r="C239" s="1">
         <v>184.03004455566406</v>
       </c>
     </row>
@@ -2773,10 +2775,10 @@
       <c r="A240" t="s">
         <v>20</v>
       </c>
-      <c r="B240" s="0">
-        <v>11</v>
-      </c>
-      <c r="C240" s="0">
+      <c r="B240" s="1">
+        <v>11</v>
+      </c>
+      <c r="C240" s="1">
         <v>214.97006225585938</v>
       </c>
     </row>
@@ -2784,10 +2786,10 @@
       <c r="A241" t="s">
         <v>20</v>
       </c>
-      <c r="B241" s="0">
-        <v>12</v>
-      </c>
-      <c r="C241" s="0">
+      <c r="B241" s="1">
+        <v>12</v>
+      </c>
+      <c r="C241" s="1">
         <v>160.72230529785156</v>
       </c>
     </row>
@@ -2795,10 +2797,10 @@
       <c r="A242" t="s">
         <v>21</v>
       </c>
-      <c r="B242" s="0">
-        <v>1</v>
-      </c>
-      <c r="C242" s="0">
+      <c r="B242" s="1">
+        <v>1</v>
+      </c>
+      <c r="C242" s="1">
         <v>123.15999603271484</v>
       </c>
     </row>
@@ -2806,10 +2808,10 @@
       <c r="A243" t="s">
         <v>21</v>
       </c>
-      <c r="B243" s="0">
-        <v>2</v>
-      </c>
-      <c r="C243" s="0">
+      <c r="B243" s="1">
+        <v>2</v>
+      </c>
+      <c r="C243" s="1">
         <v>109.74873352050781</v>
       </c>
     </row>
@@ -2817,10 +2819,10 @@
       <c r="A244" t="s">
         <v>21</v>
       </c>
-      <c r="B244" s="0">
-        <v>3</v>
-      </c>
-      <c r="C244" s="0">
+      <c r="B244" s="1">
+        <v>3</v>
+      </c>
+      <c r="C244" s="1">
         <v>116.60540008544922</v>
       </c>
     </row>
@@ -2828,10 +2830,10 @@
       <c r="A245" t="s">
         <v>21</v>
       </c>
-      <c r="B245" s="0">
-        <v>4</v>
-      </c>
-      <c r="C245" s="0">
+      <c r="B245" s="1">
+        <v>4</v>
+      </c>
+      <c r="C245" s="1">
         <v>102.28702545166016</v>
       </c>
     </row>
@@ -2839,10 +2841,10 @@
       <c r="A246" t="s">
         <v>21</v>
       </c>
-      <c r="B246" s="0">
-        <v>5</v>
-      </c>
-      <c r="C246" s="0">
+      <c r="B246" s="1">
+        <v>5</v>
+      </c>
+      <c r="C246" s="1">
         <v>121.543701171875</v>
       </c>
     </row>
@@ -2850,10 +2852,10 @@
       <c r="A247" t="s">
         <v>21</v>
       </c>
-      <c r="B247" s="0">
-        <v>6</v>
-      </c>
-      <c r="C247" s="0">
+      <c r="B247" s="1">
+        <v>6</v>
+      </c>
+      <c r="C247" s="1">
         <v>105.48676300048828</v>
       </c>
     </row>
@@ -2861,10 +2863,10 @@
       <c r="A248" t="s">
         <v>21</v>
       </c>
-      <c r="B248" s="0">
-        <v>7</v>
-      </c>
-      <c r="C248" s="0">
+      <c r="B248" s="1">
+        <v>7</v>
+      </c>
+      <c r="C248" s="1">
         <v>129.62263488769531</v>
       </c>
     </row>
@@ -2872,10 +2874,10 @@
       <c r="A249" t="s">
         <v>21</v>
       </c>
-      <c r="B249" s="0">
-        <v>8</v>
-      </c>
-      <c r="C249" s="0">
+      <c r="B249" s="1">
+        <v>8</v>
+      </c>
+      <c r="C249" s="1">
         <v>121.62975311279297</v>
       </c>
     </row>
@@ -2883,32 +2885,32 @@
       <c r="A250" t="s">
         <v>21</v>
       </c>
-      <c r="B250" s="0">
-        <v>9</v>
-      </c>
-      <c r="C250" s="0">
-        <v>157.31582641601562</v>
+      <c r="B250" s="1">
+        <v>9</v>
+      </c>
+      <c r="C250" s="1">
+        <v>157.31582641601563</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="s">
         <v>21</v>
       </c>
-      <c r="B251" s="0">
-        <v>10</v>
-      </c>
-      <c r="C251" s="0">
-        <v>183.25265502929687</v>
+      <c r="B251" s="1">
+        <v>10</v>
+      </c>
+      <c r="C251" s="1">
+        <v>183.25265502929688</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="s">
         <v>21</v>
       </c>
-      <c r="B252" s="0">
-        <v>11</v>
-      </c>
-      <c r="C252" s="0">
+      <c r="B252" s="1">
+        <v>11</v>
+      </c>
+      <c r="C252" s="1">
         <v>191.96647644042969</v>
       </c>
     </row>
@@ -2916,10 +2918,10 @@
       <c r="A253" t="s">
         <v>21</v>
       </c>
-      <c r="B253" s="0">
-        <v>12</v>
-      </c>
-      <c r="C253" s="0">
+      <c r="B253" s="1">
+        <v>12</v>
+      </c>
+      <c r="C253" s="1">
         <v>239.69102478027344</v>
       </c>
     </row>
@@ -2927,21 +2929,21 @@
       <c r="A254" t="s">
         <v>22</v>
       </c>
-      <c r="B254" s="0">
-        <v>1</v>
-      </c>
-      <c r="C254" s="0">
-        <v>309.97244262695312</v>
+      <c r="B254" s="1">
+        <v>1</v>
+      </c>
+      <c r="C254" s="1">
+        <v>309.97244262695313</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="s">
         <v>22</v>
       </c>
-      <c r="B255" s="0">
-        <v>2</v>
-      </c>
-      <c r="C255" s="0">
+      <c r="B255" s="1">
+        <v>2</v>
+      </c>
+      <c r="C255" s="1">
         <v>196.95947265625</v>
       </c>
     </row>
@@ -2949,10 +2951,10 @@
       <c r="A256" t="s">
         <v>22</v>
       </c>
-      <c r="B256" s="0">
-        <v>3</v>
-      </c>
-      <c r="C256" s="0">
+      <c r="B256" s="1">
+        <v>3</v>
+      </c>
+      <c r="C256" s="1">
         <v>212.78254699707031</v>
       </c>
     </row>
@@ -2960,10 +2962,10 @@
       <c r="A257" t="s">
         <v>22</v>
       </c>
-      <c r="B257" s="0">
-        <v>4</v>
-      </c>
-      <c r="C257" s="0">
+      <c r="B257" s="1">
+        <v>4</v>
+      </c>
+      <c r="C257" s="1">
         <v>135.51847839355469</v>
       </c>
     </row>
@@ -2971,10 +2973,10 @@
       <c r="A258" t="s">
         <v>22</v>
       </c>
-      <c r="B258" s="0">
-        <v>5</v>
-      </c>
-      <c r="C258" s="0">
+      <c r="B258" s="1">
+        <v>5</v>
+      </c>
+      <c r="C258" s="1">
         <v>158.68260192871094</v>
       </c>
     </row>
@@ -2982,10 +2984,10 @@
       <c r="A259" t="s">
         <v>22</v>
       </c>
-      <c r="B259" s="0">
-        <v>6</v>
-      </c>
-      <c r="C259" s="0">
+      <c r="B259" s="1">
+        <v>6</v>
+      </c>
+      <c r="C259" s="1">
         <v>149.80560302734375</v>
       </c>
     </row>
@@ -2993,10 +2995,10 @@
       <c r="A260" t="s">
         <v>22</v>
       </c>
-      <c r="B260" s="0">
-        <v>7</v>
-      </c>
-      <c r="C260" s="0">
+      <c r="B260" s="1">
+        <v>7</v>
+      </c>
+      <c r="C260" s="1">
         <v>202.04379272460938</v>
       </c>
     </row>
@@ -3004,10 +3006,10 @@
       <c r="A261" t="s">
         <v>22</v>
       </c>
-      <c r="B261" s="0">
-        <v>8</v>
-      </c>
-      <c r="C261" s="0">
+      <c r="B261" s="1">
+        <v>8</v>
+      </c>
+      <c r="C261" s="1">
         <v>238.91572570800781</v>
       </c>
     </row>
@@ -3015,21 +3017,21 @@
       <c r="A262" t="s">
         <v>22</v>
       </c>
-      <c r="B262" s="0">
-        <v>9</v>
-      </c>
-      <c r="C262" s="0">
-        <v>187.41012573242187</v>
+      <c r="B262" s="1">
+        <v>9</v>
+      </c>
+      <c r="C262" s="1">
+        <v>187.41012573242188</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="s">
         <v>22</v>
       </c>
-      <c r="B263" s="0">
-        <v>10</v>
-      </c>
-      <c r="C263" s="0">
+      <c r="B263" s="1">
+        <v>10</v>
+      </c>
+      <c r="C263" s="1">
         <v>233.31156921386719</v>
       </c>
     </row>
@@ -3037,10 +3039,10 @@
       <c r="A264" t="s">
         <v>22</v>
       </c>
-      <c r="B264" s="0">
-        <v>11</v>
-      </c>
-      <c r="C264" s="0">
+      <c r="B264" s="1">
+        <v>11</v>
+      </c>
+      <c r="C264" s="1">
         <v>205.59706115722656</v>
       </c>
     </row>
@@ -3048,30 +3050,41 @@
       <c r="A265" t="s">
         <v>22</v>
       </c>
-      <c r="B265" s="0">
-        <v>12</v>
-      </c>
-      <c r="C265" s="0">
-        <v>271.30404663085937</v>
+      <c r="B265" s="1">
+        <v>12</v>
+      </c>
+      <c r="C265" s="1">
+        <v>271.30404663085938</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="s">
         <v>23</v>
       </c>
-      <c r="B266" s="0">
-        <v>1</v>
-      </c>
-      <c r="C266" s="0">
-        <v>186.79362487792969</v>
+      <c r="B266" s="1">
+        <v>1</v>
+      </c>
+      <c r="C266" s="1">
+        <v>198.156494140625</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="s">
+        <v>23</v>
+      </c>
+      <c r="B267" s="1">
+        <v>2</v>
+      </c>
+      <c r="C267" s="1">
+        <v>137.52772521972656</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="s">
         <v>24</v>
       </c>
-      <c r="B267" s="0"/>
-      <c r="C267" s="0"/>
+      <c r="B268" s="1"/>
+      <c r="C268" s="1"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
update to release 2020-Q1
</commit_message>
<xml_diff>
--- a/data/epu.xlsx
+++ b/data/epu.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="27">
   <si>
     <t>year</t>
   </si>
@@ -114,7 +114,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -122,14 +122,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -139,7 +137,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C268"/>
+  <dimension ref="A1:C271"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -157,10 +155,10 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
+      <c r="B2" s="0">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0">
         <v>114.2330322265625</v>
       </c>
     </row>
@@ -168,10 +166,10 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1">
+      <c r="B3" s="0">
+        <v>2</v>
+      </c>
+      <c r="C3" s="0">
         <v>71.152473449707031</v>
       </c>
     </row>
@@ -179,10 +177,10 @@
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1">
+      <c r="B4" s="0">
+        <v>3</v>
+      </c>
+      <c r="C4" s="0">
         <v>148.08653259277344</v>
       </c>
     </row>
@@ -190,10 +188,10 @@
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="1">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1">
+      <c r="B5" s="0">
+        <v>4</v>
+      </c>
+      <c r="C5" s="0">
         <v>146.97679138183594</v>
       </c>
     </row>
@@ -201,10 +199,10 @@
       <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="1">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1">
+      <c r="B6" s="0">
+        <v>5</v>
+      </c>
+      <c r="C6" s="0">
         <v>111.51500701904297</v>
       </c>
     </row>
@@ -212,10 +210,10 @@
       <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="1">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1">
+      <c r="B7" s="0">
+        <v>6</v>
+      </c>
+      <c r="C7" s="0">
         <v>85.492919921875</v>
       </c>
     </row>
@@ -223,10 +221,10 @@
       <c r="A8" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="1">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1">
+      <c r="B8" s="0">
+        <v>7</v>
+      </c>
+      <c r="C8" s="0">
         <v>180.79301452636719</v>
       </c>
     </row>
@@ -234,10 +232,10 @@
       <c r="A9" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="1">
-        <v>8</v>
-      </c>
-      <c r="C9" s="1">
+      <c r="B9" s="0">
+        <v>8</v>
+      </c>
+      <c r="C9" s="0">
         <v>140.59883117675781</v>
       </c>
     </row>
@@ -245,10 +243,10 @@
       <c r="A10" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="1">
-        <v>9</v>
-      </c>
-      <c r="C10" s="1">
+      <c r="B10" s="0">
+        <v>9</v>
+      </c>
+      <c r="C10" s="0">
         <v>193.86285400390625</v>
       </c>
     </row>
@@ -256,21 +254,21 @@
       <c r="A11" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="1">
-        <v>10</v>
-      </c>
-      <c r="C11" s="1">
-        <v>256.06808471679688</v>
+      <c r="B11" s="0">
+        <v>10</v>
+      </c>
+      <c r="C11" s="0">
+        <v>256.06808471679687</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="1">
-        <v>11</v>
-      </c>
-      <c r="C12" s="1">
+      <c r="B12" s="0">
+        <v>11</v>
+      </c>
+      <c r="C12" s="0">
         <v>172.85871887207031</v>
       </c>
     </row>
@@ -278,10 +276,10 @@
       <c r="A13" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="1">
-        <v>12</v>
-      </c>
-      <c r="C13" s="1">
+      <c r="B13" s="0">
+        <v>12</v>
+      </c>
+      <c r="C13" s="0">
         <v>123.54463195800781</v>
       </c>
     </row>
@@ -289,10 +287,10 @@
       <c r="A14" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="1">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1">
+      <c r="B14" s="0">
+        <v>1</v>
+      </c>
+      <c r="C14" s="0">
         <v>99.624839782714844</v>
       </c>
     </row>
@@ -300,10 +298,10 @@
       <c r="A15" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="1">
-        <v>2</v>
-      </c>
-      <c r="C15" s="1">
+      <c r="B15" s="0">
+        <v>2</v>
+      </c>
+      <c r="C15" s="0">
         <v>89.3013916015625</v>
       </c>
     </row>
@@ -311,10 +309,10 @@
       <c r="A16" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="1">
-        <v>3</v>
-      </c>
-      <c r="C16" s="1">
+      <c r="B16" s="0">
+        <v>3</v>
+      </c>
+      <c r="C16" s="0">
         <v>84.704429626464844</v>
       </c>
     </row>
@@ -322,10 +320,10 @@
       <c r="A17" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="1">
-        <v>4</v>
-      </c>
-      <c r="C17" s="1">
+      <c r="B17" s="0">
+        <v>4</v>
+      </c>
+      <c r="C17" s="0">
         <v>63.930248260498047</v>
       </c>
     </row>
@@ -333,21 +331,21 @@
       <c r="A18" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="1">
-        <v>5</v>
-      </c>
-      <c r="C18" s="1">
-        <v>71.887985229492188</v>
+      <c r="B18" s="0">
+        <v>5</v>
+      </c>
+      <c r="C18" s="0">
+        <v>71.887985229492187</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="1">
-        <v>6</v>
-      </c>
-      <c r="C19" s="1">
+      <c r="B19" s="0">
+        <v>6</v>
+      </c>
+      <c r="C19" s="0">
         <v>52.256729125976563</v>
       </c>
     </row>
@@ -355,10 +353,10 @@
       <c r="A20" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="1">
-        <v>7</v>
-      </c>
-      <c r="C20" s="1">
+      <c r="B20" s="0">
+        <v>7</v>
+      </c>
+      <c r="C20" s="0">
         <v>81.232292175292969</v>
       </c>
     </row>
@@ -366,10 +364,10 @@
       <c r="A21" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="1">
-        <v>8</v>
-      </c>
-      <c r="C21" s="1">
+      <c r="B21" s="0">
+        <v>8</v>
+      </c>
+      <c r="C21" s="0">
         <v>72.576705932617188</v>
       </c>
     </row>
@@ -377,10 +375,10 @@
       <c r="A22" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="1">
-        <v>9</v>
-      </c>
-      <c r="C22" s="1">
+      <c r="B22" s="0">
+        <v>9</v>
+      </c>
+      <c r="C22" s="0">
         <v>67.1275634765625</v>
       </c>
     </row>
@@ -388,10 +386,10 @@
       <c r="A23" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="1">
-        <v>10</v>
-      </c>
-      <c r="C23" s="1">
+      <c r="B23" s="0">
+        <v>10</v>
+      </c>
+      <c r="C23" s="0">
         <v>123.12413024902344</v>
       </c>
     </row>
@@ -399,10 +397,10 @@
       <c r="A24" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="1">
-        <v>11</v>
-      </c>
-      <c r="C24" s="1">
+      <c r="B24" s="0">
+        <v>11</v>
+      </c>
+      <c r="C24" s="0">
         <v>26.846799850463867</v>
       </c>
     </row>
@@ -410,10 +408,10 @@
       <c r="A25" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="1">
-        <v>12</v>
-      </c>
-      <c r="C25" s="1">
+      <c r="B25" s="0">
+        <v>12</v>
+      </c>
+      <c r="C25" s="0">
         <v>48.689983367919922</v>
       </c>
     </row>
@@ -421,10 +419,10 @@
       <c r="A26" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="1">
-        <v>1</v>
-      </c>
-      <c r="C26" s="1">
+      <c r="B26" s="0">
+        <v>1</v>
+      </c>
+      <c r="C26" s="0">
         <v>53.748451232910156</v>
       </c>
     </row>
@@ -432,10 +430,10 @@
       <c r="A27" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="1">
-        <v>2</v>
-      </c>
-      <c r="C27" s="1">
+      <c r="B27" s="0">
+        <v>2</v>
+      </c>
+      <c r="C27" s="0">
         <v>58.396511077880859</v>
       </c>
     </row>
@@ -443,10 +441,10 @@
       <c r="A28" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="1">
-        <v>3</v>
-      </c>
-      <c r="C28" s="1">
+      <c r="B28" s="0">
+        <v>3</v>
+      </c>
+      <c r="C28" s="0">
         <v>61.960391998291016</v>
       </c>
     </row>
@@ -454,10 +452,10 @@
       <c r="A29" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="1">
-        <v>4</v>
-      </c>
-      <c r="C29" s="1">
+      <c r="B29" s="0">
+        <v>4</v>
+      </c>
+      <c r="C29" s="0">
         <v>114.01042938232422</v>
       </c>
     </row>
@@ -465,10 +463,10 @@
       <c r="A30" t="s">
         <v>3</v>
       </c>
-      <c r="B30" s="1">
-        <v>5</v>
-      </c>
-      <c r="C30" s="1">
+      <c r="B30" s="0">
+        <v>5</v>
+      </c>
+      <c r="C30" s="0">
         <v>46.368324279785156</v>
       </c>
     </row>
@@ -476,21 +474,21 @@
       <c r="A31" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="1">
-        <v>6</v>
-      </c>
-      <c r="C31" s="1">
-        <v>133.21640014648438</v>
+      <c r="B31" s="0">
+        <v>6</v>
+      </c>
+      <c r="C31" s="0">
+        <v>133.21640014648437</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="1">
-        <v>7</v>
-      </c>
-      <c r="C32" s="1">
+      <c r="B32" s="0">
+        <v>7</v>
+      </c>
+      <c r="C32" s="0">
         <v>73.706695556640625</v>
       </c>
     </row>
@@ -498,10 +496,10 @@
       <c r="A33" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="1">
-        <v>8</v>
-      </c>
-      <c r="C33" s="1">
+      <c r="B33" s="0">
+        <v>8</v>
+      </c>
+      <c r="C33" s="0">
         <v>42.748378753662109</v>
       </c>
     </row>
@@ -509,10 +507,10 @@
       <c r="A34" t="s">
         <v>3</v>
       </c>
-      <c r="B34" s="1">
-        <v>9</v>
-      </c>
-      <c r="C34" s="1">
+      <c r="B34" s="0">
+        <v>9</v>
+      </c>
+      <c r="C34" s="0">
         <v>55.577869415283203</v>
       </c>
     </row>
@@ -520,10 +518,10 @@
       <c r="A35" t="s">
         <v>3</v>
       </c>
-      <c r="B35" s="1">
-        <v>10</v>
-      </c>
-      <c r="C35" s="1">
+      <c r="B35" s="0">
+        <v>10</v>
+      </c>
+      <c r="C35" s="0">
         <v>55.821765899658203</v>
       </c>
     </row>
@@ -531,10 +529,10 @@
       <c r="A36" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="1">
-        <v>11</v>
-      </c>
-      <c r="C36" s="1">
+      <c r="B36" s="0">
+        <v>11</v>
+      </c>
+      <c r="C36" s="0">
         <v>68.99102783203125</v>
       </c>
     </row>
@@ -542,10 +540,10 @@
       <c r="A37" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="1">
-        <v>12</v>
-      </c>
-      <c r="C37" s="1">
+      <c r="B37" s="0">
+        <v>12</v>
+      </c>
+      <c r="C37" s="0">
         <v>66.450172424316406</v>
       </c>
     </row>
@@ -553,10 +551,10 @@
       <c r="A38" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="1">
-        <v>1</v>
-      </c>
-      <c r="C38" s="1">
+      <c r="B38" s="0">
+        <v>1</v>
+      </c>
+      <c r="C38" s="0">
         <v>38.407833099365234</v>
       </c>
     </row>
@@ -564,10 +562,10 @@
       <c r="A39" t="s">
         <v>4</v>
       </c>
-      <c r="B39" s="1">
-        <v>2</v>
-      </c>
-      <c r="C39" s="1">
+      <c r="B39" s="0">
+        <v>2</v>
+      </c>
+      <c r="C39" s="0">
         <v>56.693271636962891</v>
       </c>
     </row>
@@ -575,10 +573,10 @@
       <c r="A40" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="1">
-        <v>3</v>
-      </c>
-      <c r="C40" s="1">
+      <c r="B40" s="0">
+        <v>3</v>
+      </c>
+      <c r="C40" s="0">
         <v>91.642860412597656</v>
       </c>
     </row>
@@ -586,10 +584,10 @@
       <c r="A41" t="s">
         <v>4</v>
       </c>
-      <c r="B41" s="1">
-        <v>4</v>
-      </c>
-      <c r="C41" s="1">
+      <c r="B41" s="0">
+        <v>4</v>
+      </c>
+      <c r="C41" s="0">
         <v>100.98927307128906</v>
       </c>
     </row>
@@ -597,10 +595,10 @@
       <c r="A42" t="s">
         <v>4</v>
       </c>
-      <c r="B42" s="1">
-        <v>5</v>
-      </c>
-      <c r="C42" s="1">
+      <c r="B42" s="0">
+        <v>5</v>
+      </c>
+      <c r="C42" s="0">
         <v>98.2562255859375</v>
       </c>
     </row>
@@ -608,10 +606,10 @@
       <c r="A43" t="s">
         <v>4</v>
       </c>
-      <c r="B43" s="1">
-        <v>6</v>
-      </c>
-      <c r="C43" s="1">
+      <c r="B43" s="0">
+        <v>6</v>
+      </c>
+      <c r="C43" s="0">
         <v>74.842735290527344</v>
       </c>
     </row>
@@ -619,10 +617,10 @@
       <c r="A44" t="s">
         <v>4</v>
       </c>
-      <c r="B44" s="1">
-        <v>7</v>
-      </c>
-      <c r="C44" s="1">
+      <c r="B44" s="0">
+        <v>7</v>
+      </c>
+      <c r="C44" s="0">
         <v>66.38372802734375</v>
       </c>
     </row>
@@ -630,10 +628,10 @@
       <c r="A45" t="s">
         <v>4</v>
       </c>
-      <c r="B45" s="1">
-        <v>8</v>
-      </c>
-      <c r="C45" s="1">
+      <c r="B45" s="0">
+        <v>8</v>
+      </c>
+      <c r="C45" s="0">
         <v>105.13270568847656</v>
       </c>
     </row>
@@ -641,10 +639,10 @@
       <c r="A46" t="s">
         <v>4</v>
       </c>
-      <c r="B46" s="1">
-        <v>9</v>
-      </c>
-      <c r="C46" s="1">
+      <c r="B46" s="0">
+        <v>9</v>
+      </c>
+      <c r="C46" s="0">
         <v>205.25697326660156</v>
       </c>
     </row>
@@ -652,10 +650,10 @@
       <c r="A47" t="s">
         <v>4</v>
       </c>
-      <c r="B47" s="1">
-        <v>10</v>
-      </c>
-      <c r="C47" s="1">
+      <c r="B47" s="0">
+        <v>10</v>
+      </c>
+      <c r="C47" s="0">
         <v>158.72160339355469</v>
       </c>
     </row>
@@ -663,10 +661,10 @@
       <c r="A48" t="s">
         <v>4</v>
       </c>
-      <c r="B48" s="1">
-        <v>11</v>
-      </c>
-      <c r="C48" s="1">
+      <c r="B48" s="0">
+        <v>11</v>
+      </c>
+      <c r="C48" s="0">
         <v>146.11531066894531</v>
       </c>
     </row>
@@ -674,10 +672,10 @@
       <c r="A49" t="s">
         <v>4</v>
       </c>
-      <c r="B49" s="1">
-        <v>12</v>
-      </c>
-      <c r="C49" s="1">
+      <c r="B49" s="0">
+        <v>12</v>
+      </c>
+      <c r="C49" s="0">
         <v>108.11412811279297</v>
       </c>
     </row>
@@ -685,10 +683,10 @@
       <c r="A50" t="s">
         <v>5</v>
       </c>
-      <c r="B50" s="1">
-        <v>1</v>
-      </c>
-      <c r="C50" s="1">
+      <c r="B50" s="0">
+        <v>1</v>
+      </c>
+      <c r="C50" s="0">
         <v>85.506576538085938</v>
       </c>
     </row>
@@ -696,10 +694,10 @@
       <c r="A51" t="s">
         <v>5</v>
       </c>
-      <c r="B51" s="1">
-        <v>2</v>
-      </c>
-      <c r="C51" s="1">
+      <c r="B51" s="0">
+        <v>2</v>
+      </c>
+      <c r="C51" s="0">
         <v>70.793487548828125</v>
       </c>
     </row>
@@ -707,10 +705,10 @@
       <c r="A52" t="s">
         <v>5</v>
       </c>
-      <c r="B52" s="1">
-        <v>3</v>
-      </c>
-      <c r="C52" s="1">
+      <c r="B52" s="0">
+        <v>3</v>
+      </c>
+      <c r="C52" s="0">
         <v>76.328315734863281</v>
       </c>
     </row>
@@ -718,10 +716,10 @@
       <c r="A53" t="s">
         <v>5</v>
       </c>
-      <c r="B53" s="1">
-        <v>4</v>
-      </c>
-      <c r="C53" s="1">
+      <c r="B53" s="0">
+        <v>4</v>
+      </c>
+      <c r="C53" s="0">
         <v>78.088180541992188</v>
       </c>
     </row>
@@ -729,10 +727,10 @@
       <c r="A54" t="s">
         <v>5</v>
       </c>
-      <c r="B54" s="1">
-        <v>5</v>
-      </c>
-      <c r="C54" s="1">
+      <c r="B54" s="0">
+        <v>5</v>
+      </c>
+      <c r="C54" s="0">
         <v>67.406356811523438</v>
       </c>
     </row>
@@ -740,10 +738,10 @@
       <c r="A55" t="s">
         <v>5</v>
       </c>
-      <c r="B55" s="1">
-        <v>6</v>
-      </c>
-      <c r="C55" s="1">
+      <c r="B55" s="0">
+        <v>6</v>
+      </c>
+      <c r="C55" s="0">
         <v>86.87921142578125</v>
       </c>
     </row>
@@ -751,10 +749,10 @@
       <c r="A56" t="s">
         <v>5</v>
       </c>
-      <c r="B56" s="1">
-        <v>7</v>
-      </c>
-      <c r="C56" s="1">
+      <c r="B56" s="0">
+        <v>7</v>
+      </c>
+      <c r="C56" s="0">
         <v>88.472572326660156</v>
       </c>
     </row>
@@ -762,10 +760,10 @@
       <c r="A57" t="s">
         <v>5</v>
       </c>
-      <c r="B57" s="1">
-        <v>8</v>
-      </c>
-      <c r="C57" s="1">
+      <c r="B57" s="0">
+        <v>8</v>
+      </c>
+      <c r="C57" s="0">
         <v>93.7239990234375</v>
       </c>
     </row>
@@ -773,10 +771,10 @@
       <c r="A58" t="s">
         <v>5</v>
       </c>
-      <c r="B58" s="1">
-        <v>9</v>
-      </c>
-      <c r="C58" s="1">
+      <c r="B58" s="0">
+        <v>9</v>
+      </c>
+      <c r="C58" s="0">
         <v>127.27272796630859</v>
       </c>
     </row>
@@ -784,10 +782,10 @@
       <c r="A59" t="s">
         <v>5</v>
       </c>
-      <c r="B59" s="1">
-        <v>10</v>
-      </c>
-      <c r="C59" s="1">
+      <c r="B59" s="0">
+        <v>10</v>
+      </c>
+      <c r="C59" s="0">
         <v>108.42975616455078</v>
       </c>
     </row>
@@ -795,10 +793,10 @@
       <c r="A60" t="s">
         <v>5</v>
       </c>
-      <c r="B60" s="1">
-        <v>11</v>
-      </c>
-      <c r="C60" s="1">
+      <c r="B60" s="0">
+        <v>11</v>
+      </c>
+      <c r="C60" s="0">
         <v>115.09958648681641</v>
       </c>
     </row>
@@ -806,10 +804,10 @@
       <c r="A61" t="s">
         <v>5</v>
       </c>
-      <c r="B61" s="1">
-        <v>12</v>
-      </c>
-      <c r="C61" s="1">
+      <c r="B61" s="0">
+        <v>12</v>
+      </c>
+      <c r="C61" s="0">
         <v>118.64259338378906</v>
       </c>
     </row>
@@ -817,32 +815,32 @@
       <c r="A62" t="s">
         <v>6</v>
       </c>
-      <c r="B62" s="1">
-        <v>1</v>
-      </c>
-      <c r="C62" s="1">
-        <v>146.05941772460938</v>
+      <c r="B62" s="0">
+        <v>1</v>
+      </c>
+      <c r="C62" s="0">
+        <v>146.05941772460937</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
         <v>6</v>
       </c>
-      <c r="B63" s="1">
-        <v>2</v>
-      </c>
-      <c r="C63" s="1">
-        <v>178.73886108398438</v>
+      <c r="B63" s="0">
+        <v>2</v>
+      </c>
+      <c r="C63" s="0">
+        <v>178.73886108398437</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
         <v>6</v>
       </c>
-      <c r="B64" s="1">
-        <v>3</v>
-      </c>
-      <c r="C64" s="1">
+      <c r="B64" s="0">
+        <v>3</v>
+      </c>
+      <c r="C64" s="0">
         <v>174.97273254394531</v>
       </c>
     </row>
@@ -850,21 +848,21 @@
       <c r="A65" t="s">
         <v>6</v>
       </c>
-      <c r="B65" s="1">
-        <v>4</v>
-      </c>
-      <c r="C65" s="1">
-        <v>153.50643920898438</v>
+      <c r="B65" s="0">
+        <v>4</v>
+      </c>
+      <c r="C65" s="0">
+        <v>153.50643920898437</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
         <v>6</v>
       </c>
-      <c r="B66" s="1">
-        <v>5</v>
-      </c>
-      <c r="C66" s="1">
+      <c r="B66" s="0">
+        <v>5</v>
+      </c>
+      <c r="C66" s="0">
         <v>93.713760375976563</v>
       </c>
     </row>
@@ -872,10 +870,10 @@
       <c r="A67" t="s">
         <v>6</v>
       </c>
-      <c r="B67" s="1">
-        <v>6</v>
-      </c>
-      <c r="C67" s="1">
+      <c r="B67" s="0">
+        <v>6</v>
+      </c>
+      <c r="C67" s="0">
         <v>125.0064697265625</v>
       </c>
     </row>
@@ -883,10 +881,10 @@
       <c r="A68" t="s">
         <v>6</v>
       </c>
-      <c r="B68" s="1">
-        <v>7</v>
-      </c>
-      <c r="C68" s="1">
+      <c r="B68" s="0">
+        <v>7</v>
+      </c>
+      <c r="C68" s="0">
         <v>80.936637878417969</v>
       </c>
     </row>
@@ -894,10 +892,10 @@
       <c r="A69" t="s">
         <v>6</v>
       </c>
-      <c r="B69" s="1">
-        <v>8</v>
-      </c>
-      <c r="C69" s="1">
+      <c r="B69" s="0">
+        <v>8</v>
+      </c>
+      <c r="C69" s="0">
         <v>83.362625122070313</v>
       </c>
     </row>
@@ -905,10 +903,10 @@
       <c r="A70" t="s">
         <v>6</v>
       </c>
-      <c r="B70" s="1">
-        <v>9</v>
-      </c>
-      <c r="C70" s="1">
+      <c r="B70" s="0">
+        <v>9</v>
+      </c>
+      <c r="C70" s="0">
         <v>65.412857055664063</v>
       </c>
     </row>
@@ -916,10 +914,10 @@
       <c r="A71" t="s">
         <v>6</v>
       </c>
-      <c r="B71" s="1">
-        <v>10</v>
-      </c>
-      <c r="C71" s="1">
+      <c r="B71" s="0">
+        <v>10</v>
+      </c>
+      <c r="C71" s="0">
         <v>62.298290252685547</v>
       </c>
     </row>
@@ -927,10 +925,10 @@
       <c r="A72" t="s">
         <v>6</v>
       </c>
-      <c r="B72" s="1">
-        <v>11</v>
-      </c>
-      <c r="C72" s="1">
+      <c r="B72" s="0">
+        <v>11</v>
+      </c>
+      <c r="C72" s="0">
         <v>78.4478759765625</v>
       </c>
     </row>
@@ -938,10 +936,10 @@
       <c r="A73" t="s">
         <v>6</v>
       </c>
-      <c r="B73" s="1">
-        <v>12</v>
-      </c>
-      <c r="C73" s="1">
+      <c r="B73" s="0">
+        <v>12</v>
+      </c>
+      <c r="C73" s="0">
         <v>46.291194915771484</v>
       </c>
     </row>
@@ -949,10 +947,10 @@
       <c r="A74" t="s">
         <v>7</v>
       </c>
-      <c r="B74" s="1">
-        <v>1</v>
-      </c>
-      <c r="C74" s="1">
+      <c r="B74" s="0">
+        <v>1</v>
+      </c>
+      <c r="C74" s="0">
         <v>24.035942077636719</v>
       </c>
     </row>
@@ -960,10 +958,10 @@
       <c r="A75" t="s">
         <v>7</v>
       </c>
-      <c r="B75" s="1">
-        <v>2</v>
-      </c>
-      <c r="C75" s="1">
+      <c r="B75" s="0">
+        <v>2</v>
+      </c>
+      <c r="C75" s="0">
         <v>57.130153656005859</v>
       </c>
     </row>
@@ -971,10 +969,10 @@
       <c r="A76" t="s">
         <v>7</v>
       </c>
-      <c r="B76" s="1">
-        <v>3</v>
-      </c>
-      <c r="C76" s="1">
+      <c r="B76" s="0">
+        <v>3</v>
+      </c>
+      <c r="C76" s="0">
         <v>61.884700775146484</v>
       </c>
     </row>
@@ -982,10 +980,10 @@
       <c r="A77" t="s">
         <v>7</v>
       </c>
-      <c r="B77" s="1">
-        <v>4</v>
-      </c>
-      <c r="C77" s="1">
+      <c r="B77" s="0">
+        <v>4</v>
+      </c>
+      <c r="C77" s="0">
         <v>38.552352905273438</v>
       </c>
     </row>
@@ -993,10 +991,10 @@
       <c r="A78" t="s">
         <v>7</v>
       </c>
-      <c r="B78" s="1">
-        <v>5</v>
-      </c>
-      <c r="C78" s="1">
+      <c r="B78" s="0">
+        <v>5</v>
+      </c>
+      <c r="C78" s="0">
         <v>42.882164001464844</v>
       </c>
     </row>
@@ -1004,10 +1002,10 @@
       <c r="A79" t="s">
         <v>7</v>
       </c>
-      <c r="B79" s="1">
-        <v>6</v>
-      </c>
-      <c r="C79" s="1">
+      <c r="B79" s="0">
+        <v>6</v>
+      </c>
+      <c r="C79" s="0">
         <v>49.439136505126953</v>
       </c>
     </row>
@@ -1015,10 +1013,10 @@
       <c r="A80" t="s">
         <v>7</v>
       </c>
-      <c r="B80" s="1">
-        <v>7</v>
-      </c>
-      <c r="C80" s="1">
+      <c r="B80" s="0">
+        <v>7</v>
+      </c>
+      <c r="C80" s="0">
         <v>52.617275238037109</v>
       </c>
     </row>
@@ -1026,10 +1024,10 @@
       <c r="A81" t="s">
         <v>7</v>
       </c>
-      <c r="B81" s="1">
-        <v>8</v>
-      </c>
-      <c r="C81" s="1">
+      <c r="B81" s="0">
+        <v>8</v>
+      </c>
+      <c r="C81" s="0">
         <v>39.393718719482422</v>
       </c>
     </row>
@@ -1037,10 +1035,10 @@
       <c r="A82" t="s">
         <v>7</v>
       </c>
-      <c r="B82" s="1">
-        <v>9</v>
-      </c>
-      <c r="C82" s="1">
+      <c r="B82" s="0">
+        <v>9</v>
+      </c>
+      <c r="C82" s="0">
         <v>49.166225433349609</v>
       </c>
     </row>
@@ -1048,10 +1046,10 @@
       <c r="A83" t="s">
         <v>7</v>
       </c>
-      <c r="B83" s="1">
-        <v>10</v>
-      </c>
-      <c r="C83" s="1">
+      <c r="B83" s="0">
+        <v>10</v>
+      </c>
+      <c r="C83" s="0">
         <v>67.129158020019531</v>
       </c>
     </row>
@@ -1059,10 +1057,10 @@
       <c r="A84" t="s">
         <v>7</v>
       </c>
-      <c r="B84" s="1">
-        <v>11</v>
-      </c>
-      <c r="C84" s="1">
+      <c r="B84" s="0">
+        <v>11</v>
+      </c>
+      <c r="C84" s="0">
         <v>68.726028442382813</v>
       </c>
     </row>
@@ -1070,10 +1068,10 @@
       <c r="A85" t="s">
         <v>7</v>
       </c>
-      <c r="B85" s="1">
-        <v>12</v>
-      </c>
-      <c r="C85" s="1">
+      <c r="B85" s="0">
+        <v>12</v>
+      </c>
+      <c r="C85" s="0">
         <v>44.909515380859375</v>
       </c>
     </row>
@@ -1081,10 +1079,10 @@
       <c r="A86" t="s">
         <v>8</v>
       </c>
-      <c r="B86" s="1">
-        <v>1</v>
-      </c>
-      <c r="C86" s="1">
+      <c r="B86" s="0">
+        <v>1</v>
+      </c>
+      <c r="C86" s="0">
         <v>43.989646911621094</v>
       </c>
     </row>
@@ -1092,10 +1090,10 @@
       <c r="A87" t="s">
         <v>8</v>
       </c>
-      <c r="B87" s="1">
-        <v>2</v>
-      </c>
-      <c r="C87" s="1">
+      <c r="B87" s="0">
+        <v>2</v>
+      </c>
+      <c r="C87" s="0">
         <v>39.645351409912109</v>
       </c>
     </row>
@@ -1103,10 +1101,10 @@
       <c r="A88" t="s">
         <v>8</v>
       </c>
-      <c r="B88" s="1">
-        <v>3</v>
-      </c>
-      <c r="C88" s="1">
+      <c r="B88" s="0">
+        <v>3</v>
+      </c>
+      <c r="C88" s="0">
         <v>34.078708648681641</v>
       </c>
     </row>
@@ -1114,10 +1112,10 @@
       <c r="A89" t="s">
         <v>8</v>
       </c>
-      <c r="B89" s="1">
-        <v>4</v>
-      </c>
-      <c r="C89" s="1">
+      <c r="B89" s="0">
+        <v>4</v>
+      </c>
+      <c r="C89" s="0">
         <v>69.05712890625</v>
       </c>
     </row>
@@ -1125,10 +1123,10 @@
       <c r="A90" t="s">
         <v>8</v>
       </c>
-      <c r="B90" s="1">
-        <v>5</v>
-      </c>
-      <c r="C90" s="1">
+      <c r="B90" s="0">
+        <v>5</v>
+      </c>
+      <c r="C90" s="0">
         <v>71.771087646484375</v>
       </c>
     </row>
@@ -1136,10 +1134,10 @@
       <c r="A91" t="s">
         <v>8</v>
       </c>
-      <c r="B91" s="1">
-        <v>6</v>
-      </c>
-      <c r="C91" s="1">
+      <c r="B91" s="0">
+        <v>6</v>
+      </c>
+      <c r="C91" s="0">
         <v>59.403873443603516</v>
       </c>
     </row>
@@ -1147,10 +1145,10 @@
       <c r="A92" t="s">
         <v>8</v>
       </c>
-      <c r="B92" s="1">
-        <v>7</v>
-      </c>
-      <c r="C92" s="1">
+      <c r="B92" s="0">
+        <v>7</v>
+      </c>
+      <c r="C92" s="0">
         <v>47.414012908935547</v>
       </c>
     </row>
@@ -1158,10 +1156,10 @@
       <c r="A93" t="s">
         <v>8</v>
       </c>
-      <c r="B93" s="1">
-        <v>8</v>
-      </c>
-      <c r="C93" s="1">
+      <c r="B93" s="0">
+        <v>8</v>
+      </c>
+      <c r="C93" s="0">
         <v>48.541706085205078</v>
       </c>
     </row>
@@ -1169,10 +1167,10 @@
       <c r="A94" t="s">
         <v>8</v>
       </c>
-      <c r="B94" s="1">
-        <v>9</v>
-      </c>
-      <c r="C94" s="1">
+      <c r="B94" s="0">
+        <v>9</v>
+      </c>
+      <c r="C94" s="0">
         <v>70.332473754882813</v>
       </c>
     </row>
@@ -1180,10 +1178,10 @@
       <c r="A95" t="s">
         <v>8</v>
       </c>
-      <c r="B95" s="1">
-        <v>10</v>
-      </c>
-      <c r="C95" s="1">
+      <c r="B95" s="0">
+        <v>10</v>
+      </c>
+      <c r="C95" s="0">
         <v>40.613033294677734</v>
       </c>
     </row>
@@ -1191,10 +1189,10 @@
       <c r="A96" t="s">
         <v>8</v>
       </c>
-      <c r="B96" s="1">
-        <v>11</v>
-      </c>
-      <c r="C96" s="1">
+      <c r="B96" s="0">
+        <v>11</v>
+      </c>
+      <c r="C96" s="0">
         <v>47.559238433837891</v>
       </c>
     </row>
@@ -1202,10 +1200,10 @@
       <c r="A97" t="s">
         <v>8</v>
       </c>
-      <c r="B97" s="1">
-        <v>12</v>
-      </c>
-      <c r="C97" s="1">
+      <c r="B97" s="0">
+        <v>12</v>
+      </c>
+      <c r="C97" s="0">
         <v>33.106582641601563</v>
       </c>
     </row>
@@ -1213,10 +1211,10 @@
       <c r="A98" t="s">
         <v>9</v>
       </c>
-      <c r="B98" s="1">
-        <v>1</v>
-      </c>
-      <c r="C98" s="1">
+      <c r="B98" s="0">
+        <v>1</v>
+      </c>
+      <c r="C98" s="0">
         <v>44.040050506591797</v>
       </c>
     </row>
@@ -1224,10 +1222,10 @@
       <c r="A99" t="s">
         <v>9</v>
       </c>
-      <c r="B99" s="1">
-        <v>2</v>
-      </c>
-      <c r="C99" s="1">
+      <c r="B99" s="0">
+        <v>2</v>
+      </c>
+      <c r="C99" s="0">
         <v>37.132061004638672</v>
       </c>
     </row>
@@ -1235,10 +1233,10 @@
       <c r="A100" t="s">
         <v>9</v>
       </c>
-      <c r="B100" s="1">
-        <v>3</v>
-      </c>
-      <c r="C100" s="1">
+      <c r="B100" s="0">
+        <v>3</v>
+      </c>
+      <c r="C100" s="0">
         <v>42.456447601318359</v>
       </c>
     </row>
@@ -1246,10 +1244,10 @@
       <c r="A101" t="s">
         <v>9</v>
       </c>
-      <c r="B101" s="1">
-        <v>4</v>
-      </c>
-      <c r="C101" s="1">
+      <c r="B101" s="0">
+        <v>4</v>
+      </c>
+      <c r="C101" s="0">
         <v>37.08660888671875</v>
       </c>
     </row>
@@ -1257,10 +1255,10 @@
       <c r="A102" t="s">
         <v>9</v>
       </c>
-      <c r="B102" s="1">
-        <v>5</v>
-      </c>
-      <c r="C102" s="1">
+      <c r="B102" s="0">
+        <v>5</v>
+      </c>
+      <c r="C102" s="0">
         <v>74.022674560546875</v>
       </c>
     </row>
@@ -1268,10 +1266,10 @@
       <c r="A103" t="s">
         <v>9</v>
       </c>
-      <c r="B103" s="1">
-        <v>6</v>
-      </c>
-      <c r="C103" s="1">
+      <c r="B103" s="0">
+        <v>6</v>
+      </c>
+      <c r="C103" s="0">
         <v>59.820568084716797</v>
       </c>
     </row>
@@ -1279,10 +1277,10 @@
       <c r="A104" t="s">
         <v>9</v>
       </c>
-      <c r="B104" s="1">
-        <v>7</v>
-      </c>
-      <c r="C104" s="1">
+      <c r="B104" s="0">
+        <v>7</v>
+      </c>
+      <c r="C104" s="0">
         <v>47.543785095214844</v>
       </c>
     </row>
@@ -1290,10 +1288,10 @@
       <c r="A105" t="s">
         <v>9</v>
       </c>
-      <c r="B105" s="1">
-        <v>8</v>
-      </c>
-      <c r="C105" s="1">
+      <c r="B105" s="0">
+        <v>8</v>
+      </c>
+      <c r="C105" s="0">
         <v>67.213226318359375</v>
       </c>
     </row>
@@ -1301,10 +1299,10 @@
       <c r="A106" t="s">
         <v>9</v>
       </c>
-      <c r="B106" s="1">
-        <v>9</v>
-      </c>
-      <c r="C106" s="1">
+      <c r="B106" s="0">
+        <v>9</v>
+      </c>
+      <c r="C106" s="0">
         <v>56.234481811523438</v>
       </c>
     </row>
@@ -1312,21 +1310,21 @@
       <c r="A107" t="s">
         <v>9</v>
       </c>
-      <c r="B107" s="1">
-        <v>10</v>
-      </c>
-      <c r="C107" s="1">
-        <v>65.255081176757813</v>
+      <c r="B107" s="0">
+        <v>10</v>
+      </c>
+      <c r="C107" s="0">
+        <v>65.255081176757812</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
         <v>9</v>
       </c>
-      <c r="B108" s="1">
-        <v>11</v>
-      </c>
-      <c r="C108" s="1">
+      <c r="B108" s="0">
+        <v>11</v>
+      </c>
+      <c r="C108" s="0">
         <v>59.490592956542969</v>
       </c>
     </row>
@@ -1334,10 +1332,10 @@
       <c r="A109" t="s">
         <v>9</v>
       </c>
-      <c r="B109" s="1">
-        <v>12</v>
-      </c>
-      <c r="C109" s="1">
+      <c r="B109" s="0">
+        <v>12</v>
+      </c>
+      <c r="C109" s="0">
         <v>64.488700866699219</v>
       </c>
     </row>
@@ -1345,10 +1343,10 @@
       <c r="A110" t="s">
         <v>10</v>
       </c>
-      <c r="B110" s="1">
-        <v>1</v>
-      </c>
-      <c r="C110" s="1">
+      <c r="B110" s="0">
+        <v>1</v>
+      </c>
+      <c r="C110" s="0">
         <v>49.232185363769531</v>
       </c>
     </row>
@@ -1356,10 +1354,10 @@
       <c r="A111" t="s">
         <v>10</v>
       </c>
-      <c r="B111" s="1">
-        <v>2</v>
-      </c>
-      <c r="C111" s="1">
+      <c r="B111" s="0">
+        <v>2</v>
+      </c>
+      <c r="C111" s="0">
         <v>53.071933746337891</v>
       </c>
     </row>
@@ -1367,10 +1365,10 @@
       <c r="A112" t="s">
         <v>10</v>
       </c>
-      <c r="B112" s="1">
-        <v>3</v>
-      </c>
-      <c r="C112" s="1">
+      <c r="B112" s="0">
+        <v>3</v>
+      </c>
+      <c r="C112" s="0">
         <v>77.055221557617188</v>
       </c>
     </row>
@@ -1378,10 +1376,10 @@
       <c r="A113" t="s">
         <v>10</v>
       </c>
-      <c r="B113" s="1">
-        <v>4</v>
-      </c>
-      <c r="C113" s="1">
+      <c r="B113" s="0">
+        <v>4</v>
+      </c>
+      <c r="C113" s="0">
         <v>60.96484375</v>
       </c>
     </row>
@@ -1389,10 +1387,10 @@
       <c r="A114" t="s">
         <v>10</v>
       </c>
-      <c r="B114" s="1">
-        <v>5</v>
-      </c>
-      <c r="C114" s="1">
+      <c r="B114" s="0">
+        <v>5</v>
+      </c>
+      <c r="C114" s="0">
         <v>66.573944091796875</v>
       </c>
     </row>
@@ -1400,10 +1398,10 @@
       <c r="A115" t="s">
         <v>10</v>
       </c>
-      <c r="B115" s="1">
-        <v>6</v>
-      </c>
-      <c r="C115" s="1">
+      <c r="B115" s="0">
+        <v>6</v>
+      </c>
+      <c r="C115" s="0">
         <v>53.468608856201172</v>
       </c>
     </row>
@@ -1411,10 +1409,10 @@
       <c r="A116" t="s">
         <v>10</v>
       </c>
-      <c r="B116" s="1">
-        <v>7</v>
-      </c>
-      <c r="C116" s="1">
+      <c r="B116" s="0">
+        <v>7</v>
+      </c>
+      <c r="C116" s="0">
         <v>48.757678985595703</v>
       </c>
     </row>
@@ -1422,10 +1420,10 @@
       <c r="A117" t="s">
         <v>10</v>
       </c>
-      <c r="B117" s="1">
-        <v>8</v>
-      </c>
-      <c r="C117" s="1">
+      <c r="B117" s="0">
+        <v>8</v>
+      </c>
+      <c r="C117" s="0">
         <v>77.388679504394531</v>
       </c>
     </row>
@@ -1433,10 +1431,10 @@
       <c r="A118" t="s">
         <v>10</v>
       </c>
-      <c r="B118" s="1">
-        <v>9</v>
-      </c>
-      <c r="C118" s="1">
+      <c r="B118" s="0">
+        <v>9</v>
+      </c>
+      <c r="C118" s="0">
         <v>132.26576232910156</v>
       </c>
     </row>
@@ -1444,10 +1442,10 @@
       <c r="A119" t="s">
         <v>10</v>
       </c>
-      <c r="B119" s="1">
-        <v>10</v>
-      </c>
-      <c r="C119" s="1">
+      <c r="B119" s="0">
+        <v>10</v>
+      </c>
+      <c r="C119" s="0">
         <v>91.692916870117188</v>
       </c>
     </row>
@@ -1455,10 +1453,10 @@
       <c r="A120" t="s">
         <v>10</v>
       </c>
-      <c r="B120" s="1">
-        <v>11</v>
-      </c>
-      <c r="C120" s="1">
+      <c r="B120" s="0">
+        <v>11</v>
+      </c>
+      <c r="C120" s="0">
         <v>131.62321472167969</v>
       </c>
     </row>
@@ -1466,10 +1464,10 @@
       <c r="A121" t="s">
         <v>10</v>
       </c>
-      <c r="B121" s="1">
-        <v>12</v>
-      </c>
-      <c r="C121" s="1">
+      <c r="B121" s="0">
+        <v>12</v>
+      </c>
+      <c r="C121" s="0">
         <v>150.87321472167969</v>
       </c>
     </row>
@@ -1477,10 +1475,10 @@
       <c r="A122" t="s">
         <v>11</v>
       </c>
-      <c r="B122" s="1">
-        <v>1</v>
-      </c>
-      <c r="C122" s="1">
+      <c r="B122" s="0">
+        <v>1</v>
+      </c>
+      <c r="C122" s="0">
         <v>138.57289123535156</v>
       </c>
     </row>
@@ -1488,32 +1486,32 @@
       <c r="A123" t="s">
         <v>11</v>
       </c>
-      <c r="B123" s="1">
-        <v>2</v>
-      </c>
-      <c r="C123" s="1">
-        <v>145.78488159179688</v>
+      <c r="B123" s="0">
+        <v>2</v>
+      </c>
+      <c r="C123" s="0">
+        <v>145.78488159179687</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="s">
         <v>11</v>
       </c>
-      <c r="B124" s="1">
-        <v>3</v>
-      </c>
-      <c r="C124" s="1">
-        <v>168.74942016601563</v>
+      <c r="B124" s="0">
+        <v>3</v>
+      </c>
+      <c r="C124" s="0">
+        <v>168.74942016601562</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="s">
         <v>11</v>
       </c>
-      <c r="B125" s="1">
-        <v>4</v>
-      </c>
-      <c r="C125" s="1">
+      <c r="B125" s="0">
+        <v>4</v>
+      </c>
+      <c r="C125" s="0">
         <v>129.51087951660156</v>
       </c>
     </row>
@@ -1521,10 +1519,10 @@
       <c r="A126" t="s">
         <v>11</v>
       </c>
-      <c r="B126" s="1">
-        <v>5</v>
-      </c>
-      <c r="C126" s="1">
+      <c r="B126" s="0">
+        <v>5</v>
+      </c>
+      <c r="C126" s="0">
         <v>112.51808166503906</v>
       </c>
     </row>
@@ -1532,10 +1530,10 @@
       <c r="A127" t="s">
         <v>11</v>
       </c>
-      <c r="B127" s="1">
-        <v>6</v>
-      </c>
-      <c r="C127" s="1">
+      <c r="B127" s="0">
+        <v>6</v>
+      </c>
+      <c r="C127" s="0">
         <v>107.00999450683594</v>
       </c>
     </row>
@@ -1543,10 +1541,10 @@
       <c r="A128" t="s">
         <v>11</v>
       </c>
-      <c r="B128" s="1">
-        <v>7</v>
-      </c>
-      <c r="C128" s="1">
+      <c r="B128" s="0">
+        <v>7</v>
+      </c>
+      <c r="C128" s="0">
         <v>113.38642883300781</v>
       </c>
     </row>
@@ -1554,10 +1552,10 @@
       <c r="A129" t="s">
         <v>11</v>
       </c>
-      <c r="B129" s="1">
-        <v>8</v>
-      </c>
-      <c r="C129" s="1">
+      <c r="B129" s="0">
+        <v>8</v>
+      </c>
+      <c r="C129" s="0">
         <v>143.64463806152344</v>
       </c>
     </row>
@@ -1565,10 +1563,10 @@
       <c r="A130" t="s">
         <v>11</v>
       </c>
-      <c r="B130" s="1">
-        <v>9</v>
-      </c>
-      <c r="C130" s="1">
+      <c r="B130" s="0">
+        <v>9</v>
+      </c>
+      <c r="C130" s="0">
         <v>191.05964660644531</v>
       </c>
     </row>
@@ -1576,10 +1574,10 @@
       <c r="A131" t="s">
         <v>11</v>
       </c>
-      <c r="B131" s="1">
-        <v>10</v>
-      </c>
-      <c r="C131" s="1">
+      <c r="B131" s="0">
+        <v>10</v>
+      </c>
+      <c r="C131" s="0">
         <v>242.234375</v>
       </c>
     </row>
@@ -1587,21 +1585,21 @@
       <c r="A132" t="s">
         <v>11</v>
       </c>
-      <c r="B132" s="1">
-        <v>11</v>
-      </c>
-      <c r="C132" s="1">
-        <v>169.54904174804688</v>
+      <c r="B132" s="0">
+        <v>11</v>
+      </c>
+      <c r="C132" s="0">
+        <v>169.54904174804687</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="s">
         <v>11</v>
       </c>
-      <c r="B133" s="1">
-        <v>12</v>
-      </c>
-      <c r="C133" s="1">
+      <c r="B133" s="0">
+        <v>12</v>
+      </c>
+      <c r="C133" s="0">
         <v>123.49229431152344</v>
       </c>
     </row>
@@ -1609,10 +1607,10 @@
       <c r="A134" t="s">
         <v>12</v>
       </c>
-      <c r="B134" s="1">
-        <v>1</v>
-      </c>
-      <c r="C134" s="1">
+      <c r="B134" s="0">
+        <v>1</v>
+      </c>
+      <c r="C134" s="0">
         <v>129.44589233398438</v>
       </c>
     </row>
@@ -1620,21 +1618,21 @@
       <c r="A135" t="s">
         <v>12</v>
       </c>
-      <c r="B135" s="1">
-        <v>2</v>
-      </c>
-      <c r="C135" s="1">
-        <v>129.95285034179688</v>
+      <c r="B135" s="0">
+        <v>2</v>
+      </c>
+      <c r="C135" s="0">
+        <v>129.95285034179687</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="s">
         <v>12</v>
       </c>
-      <c r="B136" s="1">
-        <v>3</v>
-      </c>
-      <c r="C136" s="1">
+      <c r="B136" s="0">
+        <v>3</v>
+      </c>
+      <c r="C136" s="0">
         <v>111.89681243896484</v>
       </c>
     </row>
@@ -1642,10 +1640,10 @@
       <c r="A137" t="s">
         <v>12</v>
       </c>
-      <c r="B137" s="1">
-        <v>4</v>
-      </c>
-      <c r="C137" s="1">
+      <c r="B137" s="0">
+        <v>4</v>
+      </c>
+      <c r="C137" s="0">
         <v>111.6890869140625</v>
       </c>
     </row>
@@ -1653,10 +1651,10 @@
       <c r="A138" t="s">
         <v>12</v>
       </c>
-      <c r="B138" s="1">
-        <v>5</v>
-      </c>
-      <c r="C138" s="1">
+      <c r="B138" s="0">
+        <v>5</v>
+      </c>
+      <c r="C138" s="0">
         <v>116.61088562011719</v>
       </c>
     </row>
@@ -1664,21 +1662,21 @@
       <c r="A139" t="s">
         <v>12</v>
       </c>
-      <c r="B139" s="1">
-        <v>6</v>
-      </c>
-      <c r="C139" s="1">
-        <v>154.18637084960938</v>
+      <c r="B139" s="0">
+        <v>6</v>
+      </c>
+      <c r="C139" s="0">
+        <v>154.18637084960937</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="s">
         <v>12</v>
       </c>
-      <c r="B140" s="1">
-        <v>7</v>
-      </c>
-      <c r="C140" s="1">
+      <c r="B140" s="0">
+        <v>7</v>
+      </c>
+      <c r="C140" s="0">
         <v>128.96145629882813</v>
       </c>
     </row>
@@ -1686,21 +1684,21 @@
       <c r="A141" t="s">
         <v>12</v>
       </c>
-      <c r="B141" s="1">
-        <v>8</v>
-      </c>
-      <c r="C141" s="1">
-        <v>117.74832153320313</v>
+      <c r="B141" s="0">
+        <v>8</v>
+      </c>
+      <c r="C141" s="0">
+        <v>117.74832153320312</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="s">
         <v>12</v>
       </c>
-      <c r="B142" s="1">
-        <v>9</v>
-      </c>
-      <c r="C142" s="1">
+      <c r="B142" s="0">
+        <v>9</v>
+      </c>
+      <c r="C142" s="0">
         <v>100.07635498046875</v>
       </c>
     </row>
@@ -1708,10 +1706,10 @@
       <c r="A143" t="s">
         <v>12</v>
       </c>
-      <c r="B143" s="1">
-        <v>10</v>
-      </c>
-      <c r="C143" s="1">
+      <c r="B143" s="0">
+        <v>10</v>
+      </c>
+      <c r="C143" s="0">
         <v>107.54240417480469</v>
       </c>
     </row>
@@ -1719,10 +1717,10 @@
       <c r="A144" t="s">
         <v>12</v>
       </c>
-      <c r="B144" s="1">
-        <v>11</v>
-      </c>
-      <c r="C144" s="1">
+      <c r="B144" s="0">
+        <v>11</v>
+      </c>
+      <c r="C144" s="0">
         <v>107.57199859619141</v>
       </c>
     </row>
@@ -1730,10 +1728,10 @@
       <c r="A145" t="s">
         <v>12</v>
       </c>
-      <c r="B145" s="1">
-        <v>12</v>
-      </c>
-      <c r="C145" s="1">
+      <c r="B145" s="0">
+        <v>12</v>
+      </c>
+      <c r="C145" s="0">
         <v>135.97782897949219</v>
       </c>
     </row>
@@ -1741,10 +1739,10 @@
       <c r="A146" t="s">
         <v>13</v>
       </c>
-      <c r="B146" s="1">
-        <v>1</v>
-      </c>
-      <c r="C146" s="1">
+      <c r="B146" s="0">
+        <v>1</v>
+      </c>
+      <c r="C146" s="0">
         <v>148.26554870605469</v>
       </c>
     </row>
@@ -1752,10 +1750,10 @@
       <c r="A147" t="s">
         <v>13</v>
       </c>
-      <c r="B147" s="1">
-        <v>2</v>
-      </c>
-      <c r="C147" s="1">
+      <c r="B147" s="0">
+        <v>2</v>
+      </c>
+      <c r="C147" s="0">
         <v>143.34239196777344</v>
       </c>
     </row>
@@ -1763,10 +1761,10 @@
       <c r="A148" t="s">
         <v>13</v>
       </c>
-      <c r="B148" s="1">
-        <v>3</v>
-      </c>
-      <c r="C148" s="1">
+      <c r="B148" s="0">
+        <v>3</v>
+      </c>
+      <c r="C148" s="0">
         <v>160.08869934082031</v>
       </c>
     </row>
@@ -1774,10 +1772,10 @@
       <c r="A149" t="s">
         <v>13</v>
       </c>
-      <c r="B149" s="1">
-        <v>4</v>
-      </c>
-      <c r="C149" s="1">
+      <c r="B149" s="0">
+        <v>4</v>
+      </c>
+      <c r="C149" s="0">
         <v>161.00445556640625</v>
       </c>
     </row>
@@ -1785,10 +1783,10 @@
       <c r="A150" t="s">
         <v>13</v>
       </c>
-      <c r="B150" s="1">
-        <v>5</v>
-      </c>
-      <c r="C150" s="1">
+      <c r="B150" s="0">
+        <v>5</v>
+      </c>
+      <c r="C150" s="0">
         <v>243.53857421875</v>
       </c>
     </row>
@@ -1796,21 +1794,21 @@
       <c r="A151" t="s">
         <v>13</v>
       </c>
-      <c r="B151" s="1">
-        <v>6</v>
-      </c>
-      <c r="C151" s="1">
-        <v>184.01828002929688</v>
+      <c r="B151" s="0">
+        <v>6</v>
+      </c>
+      <c r="C151" s="0">
+        <v>184.01828002929687</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="s">
         <v>13</v>
       </c>
-      <c r="B152" s="1">
-        <v>7</v>
-      </c>
-      <c r="C152" s="1">
+      <c r="B152" s="0">
+        <v>7</v>
+      </c>
+      <c r="C152" s="0">
         <v>142.86163330078125</v>
       </c>
     </row>
@@ -1818,21 +1816,21 @@
       <c r="A153" t="s">
         <v>13</v>
       </c>
-      <c r="B153" s="1">
-        <v>8</v>
-      </c>
-      <c r="C153" s="1">
-        <v>165.98422241210938</v>
+      <c r="B153" s="0">
+        <v>8</v>
+      </c>
+      <c r="C153" s="0">
+        <v>165.98422241210937</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="s">
         <v>13</v>
       </c>
-      <c r="B154" s="1">
-        <v>9</v>
-      </c>
-      <c r="C154" s="1">
+      <c r="B154" s="0">
+        <v>9</v>
+      </c>
+      <c r="C154" s="0">
         <v>127.90261840820313</v>
       </c>
     </row>
@@ -1840,10 +1838,10 @@
       <c r="A155" t="s">
         <v>13</v>
       </c>
-      <c r="B155" s="1">
-        <v>10</v>
-      </c>
-      <c r="C155" s="1">
+      <c r="B155" s="0">
+        <v>10</v>
+      </c>
+      <c r="C155" s="0">
         <v>177.80287170410156</v>
       </c>
     </row>
@@ -1851,10 +1849,10 @@
       <c r="A156" t="s">
         <v>13</v>
       </c>
-      <c r="B156" s="1">
-        <v>11</v>
-      </c>
-      <c r="C156" s="1">
+      <c r="B156" s="0">
+        <v>11</v>
+      </c>
+      <c r="C156" s="0">
         <v>153.24842834472656</v>
       </c>
     </row>
@@ -1862,10 +1860,10 @@
       <c r="A157" t="s">
         <v>13</v>
       </c>
-      <c r="B157" s="1">
-        <v>12</v>
-      </c>
-      <c r="C157" s="1">
+      <c r="B157" s="0">
+        <v>12</v>
+      </c>
+      <c r="C157" s="0">
         <v>122.77899169921875</v>
       </c>
     </row>
@@ -1873,21 +1871,21 @@
       <c r="A158" t="s">
         <v>14</v>
       </c>
-      <c r="B158" s="1">
-        <v>1</v>
-      </c>
-      <c r="C158" s="1">
-        <v>123.68014526367188</v>
+      <c r="B158" s="0">
+        <v>1</v>
+      </c>
+      <c r="C158" s="0">
+        <v>123.68014526367187</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="s">
         <v>14</v>
       </c>
-      <c r="B159" s="1">
-        <v>2</v>
-      </c>
-      <c r="C159" s="1">
+      <c r="B159" s="0">
+        <v>2</v>
+      </c>
+      <c r="C159" s="0">
         <v>119.12128448486328</v>
       </c>
     </row>
@@ -1895,10 +1893,10 @@
       <c r="A160" t="s">
         <v>14</v>
       </c>
-      <c r="B160" s="1">
-        <v>3</v>
-      </c>
-      <c r="C160" s="1">
+      <c r="B160" s="0">
+        <v>3</v>
+      </c>
+      <c r="C160" s="0">
         <v>131.42254638671875</v>
       </c>
     </row>
@@ -1906,10 +1904,10 @@
       <c r="A161" t="s">
         <v>14</v>
       </c>
-      <c r="B161" s="1">
-        <v>4</v>
-      </c>
-      <c r="C161" s="1">
+      <c r="B161" s="0">
+        <v>4</v>
+      </c>
+      <c r="C161" s="0">
         <v>97.936988830566406</v>
       </c>
     </row>
@@ -1917,10 +1915,10 @@
       <c r="A162" t="s">
         <v>14</v>
       </c>
-      <c r="B162" s="1">
-        <v>5</v>
-      </c>
-      <c r="C162" s="1">
+      <c r="B162" s="0">
+        <v>5</v>
+      </c>
+      <c r="C162" s="0">
         <v>94.244071960449219</v>
       </c>
     </row>
@@ -1928,10 +1926,10 @@
       <c r="A163" t="s">
         <v>14</v>
       </c>
-      <c r="B163" s="1">
-        <v>6</v>
-      </c>
-      <c r="C163" s="1">
+      <c r="B163" s="0">
+        <v>6</v>
+      </c>
+      <c r="C163" s="0">
         <v>122.69766998291016</v>
       </c>
     </row>
@@ -1939,21 +1937,21 @@
       <c r="A164" t="s">
         <v>14</v>
       </c>
-      <c r="B164" s="1">
-        <v>7</v>
-      </c>
-      <c r="C164" s="1">
-        <v>149.02828979492188</v>
+      <c r="B164" s="0">
+        <v>7</v>
+      </c>
+      <c r="C164" s="0">
+        <v>149.02828979492187</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="s">
         <v>14</v>
       </c>
-      <c r="B165" s="1">
-        <v>8</v>
-      </c>
-      <c r="C165" s="1">
+      <c r="B165" s="0">
+        <v>8</v>
+      </c>
+      <c r="C165" s="0">
         <v>177.75312805175781</v>
       </c>
     </row>
@@ -1961,10 +1959,10 @@
       <c r="A166" t="s">
         <v>14</v>
       </c>
-      <c r="B166" s="1">
-        <v>9</v>
-      </c>
-      <c r="C166" s="1">
+      <c r="B166" s="0">
+        <v>9</v>
+      </c>
+      <c r="C166" s="0">
         <v>153.32763671875</v>
       </c>
     </row>
@@ -1972,10 +1970,10 @@
       <c r="A167" t="s">
         <v>14</v>
       </c>
-      <c r="B167" s="1">
-        <v>10</v>
-      </c>
-      <c r="C167" s="1">
+      <c r="B167" s="0">
+        <v>10</v>
+      </c>
+      <c r="C167" s="0">
         <v>149.69090270996094</v>
       </c>
     </row>
@@ -1983,10 +1981,10 @@
       <c r="A168" t="s">
         <v>14</v>
       </c>
-      <c r="B168" s="1">
-        <v>11</v>
-      </c>
-      <c r="C168" s="1">
+      <c r="B168" s="0">
+        <v>11</v>
+      </c>
+      <c r="C168" s="0">
         <v>209.89849853515625</v>
       </c>
     </row>
@@ -1994,10 +1992,10 @@
       <c r="A169" t="s">
         <v>14</v>
       </c>
-      <c r="B169" s="1">
-        <v>12</v>
-      </c>
-      <c r="C169" s="1">
+      <c r="B169" s="0">
+        <v>12</v>
+      </c>
+      <c r="C169" s="0">
         <v>140.62797546386719</v>
       </c>
     </row>
@@ -2005,10 +2003,10 @@
       <c r="A170" t="s">
         <v>15</v>
       </c>
-      <c r="B170" s="1">
-        <v>1</v>
-      </c>
-      <c r="C170" s="1">
+      <c r="B170" s="0">
+        <v>1</v>
+      </c>
+      <c r="C170" s="0">
         <v>137.26155090332031</v>
       </c>
     </row>
@@ -2016,10 +2014,10 @@
       <c r="A171" t="s">
         <v>15</v>
       </c>
-      <c r="B171" s="1">
-        <v>2</v>
-      </c>
-      <c r="C171" s="1">
+      <c r="B171" s="0">
+        <v>2</v>
+      </c>
+      <c r="C171" s="0">
         <v>132.02021789550781</v>
       </c>
     </row>
@@ -2027,10 +2025,10 @@
       <c r="A172" t="s">
         <v>15</v>
       </c>
-      <c r="B172" s="1">
-        <v>3</v>
-      </c>
-      <c r="C172" s="1">
+      <c r="B172" s="0">
+        <v>3</v>
+      </c>
+      <c r="C172" s="0">
         <v>103.72963714599609</v>
       </c>
     </row>
@@ -2038,10 +2036,10 @@
       <c r="A173" t="s">
         <v>15</v>
       </c>
-      <c r="B173" s="1">
-        <v>4</v>
-      </c>
-      <c r="C173" s="1">
+      <c r="B173" s="0">
+        <v>4</v>
+      </c>
+      <c r="C173" s="0">
         <v>109.31269073486328</v>
       </c>
     </row>
@@ -2049,10 +2047,10 @@
       <c r="A174" t="s">
         <v>15</v>
       </c>
-      <c r="B174" s="1">
-        <v>5</v>
-      </c>
-      <c r="C174" s="1">
+      <c r="B174" s="0">
+        <v>5</v>
+      </c>
+      <c r="C174" s="0">
         <v>151.78517150878906</v>
       </c>
     </row>
@@ -2060,10 +2058,10 @@
       <c r="A175" t="s">
         <v>15</v>
       </c>
-      <c r="B175" s="1">
-        <v>6</v>
-      </c>
-      <c r="C175" s="1">
+      <c r="B175" s="0">
+        <v>6</v>
+      </c>
+      <c r="C175" s="0">
         <v>169.64906311035156</v>
       </c>
     </row>
@@ -2071,10 +2069,10 @@
       <c r="A176" t="s">
         <v>15</v>
       </c>
-      <c r="B176" s="1">
-        <v>7</v>
-      </c>
-      <c r="C176" s="1">
+      <c r="B176" s="0">
+        <v>7</v>
+      </c>
+      <c r="C176" s="0">
         <v>129.98323059082031</v>
       </c>
     </row>
@@ -2082,10 +2080,10 @@
       <c r="A177" t="s">
         <v>15</v>
       </c>
-      <c r="B177" s="1">
-        <v>8</v>
-      </c>
-      <c r="C177" s="1">
+      <c r="B177" s="0">
+        <v>8</v>
+      </c>
+      <c r="C177" s="0">
         <v>98.178688049316406</v>
       </c>
     </row>
@@ -2093,10 +2091,10 @@
       <c r="A178" t="s">
         <v>15</v>
       </c>
-      <c r="B178" s="1">
-        <v>9</v>
-      </c>
-      <c r="C178" s="1">
+      <c r="B178" s="0">
+        <v>9</v>
+      </c>
+      <c r="C178" s="0">
         <v>124.43543243408203</v>
       </c>
     </row>
@@ -2104,21 +2102,21 @@
       <c r="A179" t="s">
         <v>15</v>
       </c>
-      <c r="B179" s="1">
-        <v>10</v>
-      </c>
-      <c r="C179" s="1">
-        <v>153.99227905273438</v>
+      <c r="B179" s="0">
+        <v>10</v>
+      </c>
+      <c r="C179" s="0">
+        <v>153.99227905273437</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="s">
         <v>15</v>
       </c>
-      <c r="B180" s="1">
-        <v>11</v>
-      </c>
-      <c r="C180" s="1">
+      <c r="B180" s="0">
+        <v>11</v>
+      </c>
+      <c r="C180" s="0">
         <v>162.10096740722656</v>
       </c>
     </row>
@@ -2126,10 +2124,10 @@
       <c r="A181" t="s">
         <v>15</v>
       </c>
-      <c r="B181" s="1">
-        <v>12</v>
-      </c>
-      <c r="C181" s="1">
+      <c r="B181" s="0">
+        <v>12</v>
+      </c>
+      <c r="C181" s="0">
         <v>140.64390563964844</v>
       </c>
     </row>
@@ -2137,21 +2135,21 @@
       <c r="A182" t="s">
         <v>16</v>
       </c>
-      <c r="B182" s="1">
-        <v>1</v>
-      </c>
-      <c r="C182" s="1">
-        <v>187.77023315429688</v>
+      <c r="B182" s="0">
+        <v>1</v>
+      </c>
+      <c r="C182" s="0">
+        <v>187.77023315429687</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="s">
         <v>16</v>
       </c>
-      <c r="B183" s="1">
-        <v>2</v>
-      </c>
-      <c r="C183" s="1">
+      <c r="B183" s="0">
+        <v>2</v>
+      </c>
+      <c r="C183" s="0">
         <v>97.381301879882813</v>
       </c>
     </row>
@@ -2159,21 +2157,21 @@
       <c r="A184" t="s">
         <v>16</v>
       </c>
-      <c r="B184" s="1">
-        <v>3</v>
-      </c>
-      <c r="C184" s="1">
-        <v>108.96334838867188</v>
+      <c r="B184" s="0">
+        <v>3</v>
+      </c>
+      <c r="C184" s="0">
+        <v>108.96334838867187</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="s">
         <v>16</v>
       </c>
-      <c r="B185" s="1">
-        <v>4</v>
-      </c>
-      <c r="C185" s="1">
+      <c r="B185" s="0">
+        <v>4</v>
+      </c>
+      <c r="C185" s="0">
         <v>101.40814971923828</v>
       </c>
     </row>
@@ -2181,10 +2179,10 @@
       <c r="A186" t="s">
         <v>16</v>
       </c>
-      <c r="B186" s="1">
-        <v>5</v>
-      </c>
-      <c r="C186" s="1">
+      <c r="B186" s="0">
+        <v>5</v>
+      </c>
+      <c r="C186" s="0">
         <v>72.982437133789063</v>
       </c>
     </row>
@@ -2192,10 +2190,10 @@
       <c r="A187" t="s">
         <v>16</v>
       </c>
-      <c r="B187" s="1">
-        <v>6</v>
-      </c>
-      <c r="C187" s="1">
+      <c r="B187" s="0">
+        <v>6</v>
+      </c>
+      <c r="C187" s="0">
         <v>90.508140563964844</v>
       </c>
     </row>
@@ -2203,10 +2201,10 @@
       <c r="A188" t="s">
         <v>16</v>
       </c>
-      <c r="B188" s="1">
-        <v>7</v>
-      </c>
-      <c r="C188" s="1">
+      <c r="B188" s="0">
+        <v>7</v>
+      </c>
+      <c r="C188" s="0">
         <v>68.187995910644531</v>
       </c>
     </row>
@@ -2214,10 +2212,10 @@
       <c r="A189" t="s">
         <v>16</v>
       </c>
-      <c r="B189" s="1">
-        <v>8</v>
-      </c>
-      <c r="C189" s="1">
+      <c r="B189" s="0">
+        <v>8</v>
+      </c>
+      <c r="C189" s="0">
         <v>91.647727966308594</v>
       </c>
     </row>
@@ -2225,10 +2223,10 @@
       <c r="A190" t="s">
         <v>16</v>
       </c>
-      <c r="B190" s="1">
-        <v>9</v>
-      </c>
-      <c r="C190" s="1">
+      <c r="B190" s="0">
+        <v>9</v>
+      </c>
+      <c r="C190" s="0">
         <v>94.262176513671875</v>
       </c>
     </row>
@@ -2236,10 +2234,10 @@
       <c r="A191" t="s">
         <v>16</v>
       </c>
-      <c r="B191" s="1">
-        <v>10</v>
-      </c>
-      <c r="C191" s="1">
+      <c r="B191" s="0">
+        <v>10</v>
+      </c>
+      <c r="C191" s="0">
         <v>110.99637603759766</v>
       </c>
     </row>
@@ -2247,10 +2245,10 @@
       <c r="A192" t="s">
         <v>16</v>
       </c>
-      <c r="B192" s="1">
-        <v>11</v>
-      </c>
-      <c r="C192" s="1">
+      <c r="B192" s="0">
+        <v>11</v>
+      </c>
+      <c r="C192" s="0">
         <v>82.074790954589844</v>
       </c>
     </row>
@@ -2258,10 +2256,10 @@
       <c r="A193" t="s">
         <v>16</v>
       </c>
-      <c r="B193" s="1">
-        <v>12</v>
-      </c>
-      <c r="C193" s="1">
+      <c r="B193" s="0">
+        <v>12</v>
+      </c>
+      <c r="C193" s="0">
         <v>89.423934936523438</v>
       </c>
     </row>
@@ -2269,10 +2267,10 @@
       <c r="A194" t="s">
         <v>17</v>
       </c>
-      <c r="B194" s="1">
-        <v>1</v>
-      </c>
-      <c r="C194" s="1">
+      <c r="B194" s="0">
+        <v>1</v>
+      </c>
+      <c r="C194" s="0">
         <v>103.99873352050781</v>
       </c>
     </row>
@@ -2280,10 +2278,10 @@
       <c r="A195" t="s">
         <v>17</v>
       </c>
-      <c r="B195" s="1">
-        <v>2</v>
-      </c>
-      <c r="C195" s="1">
+      <c r="B195" s="0">
+        <v>2</v>
+      </c>
+      <c r="C195" s="0">
         <v>117.69552612304688</v>
       </c>
     </row>
@@ -2291,10 +2289,10 @@
       <c r="A196" t="s">
         <v>17</v>
       </c>
-      <c r="B196" s="1">
-        <v>3</v>
-      </c>
-      <c r="C196" s="1">
+      <c r="B196" s="0">
+        <v>3</v>
+      </c>
+      <c r="C196" s="0">
         <v>111.04788970947266</v>
       </c>
     </row>
@@ -2302,10 +2300,10 @@
       <c r="A197" t="s">
         <v>17</v>
       </c>
-      <c r="B197" s="1">
-        <v>4</v>
-      </c>
-      <c r="C197" s="1">
+      <c r="B197" s="0">
+        <v>4</v>
+      </c>
+      <c r="C197" s="0">
         <v>71.126228332519531</v>
       </c>
     </row>
@@ -2313,10 +2311,10 @@
       <c r="A198" t="s">
         <v>17</v>
       </c>
-      <c r="B198" s="1">
-        <v>5</v>
-      </c>
-      <c r="C198" s="1">
+      <c r="B198" s="0">
+        <v>5</v>
+      </c>
+      <c r="C198" s="0">
         <v>90.164924621582031</v>
       </c>
     </row>
@@ -2324,10 +2322,10 @@
       <c r="A199" t="s">
         <v>17</v>
       </c>
-      <c r="B199" s="1">
-        <v>6</v>
-      </c>
-      <c r="C199" s="1">
+      <c r="B199" s="0">
+        <v>6</v>
+      </c>
+      <c r="C199" s="0">
         <v>68.777374267578125</v>
       </c>
     </row>
@@ -2335,10 +2333,10 @@
       <c r="A200" t="s">
         <v>17</v>
       </c>
-      <c r="B200" s="1">
-        <v>7</v>
-      </c>
-      <c r="C200" s="1">
+      <c r="B200" s="0">
+        <v>7</v>
+      </c>
+      <c r="C200" s="0">
         <v>62.335445404052734</v>
       </c>
     </row>
@@ -2346,10 +2344,10 @@
       <c r="A201" t="s">
         <v>17</v>
       </c>
-      <c r="B201" s="1">
-        <v>8</v>
-      </c>
-      <c r="C201" s="1">
+      <c r="B201" s="0">
+        <v>8</v>
+      </c>
+      <c r="C201" s="0">
         <v>132.47334289550781</v>
       </c>
     </row>
@@ -2357,21 +2355,21 @@
       <c r="A202" t="s">
         <v>17</v>
       </c>
-      <c r="B202" s="1">
-        <v>9</v>
-      </c>
-      <c r="C202" s="1">
-        <v>176.28372192382813</v>
+      <c r="B202" s="0">
+        <v>9</v>
+      </c>
+      <c r="C202" s="0">
+        <v>176.28372192382812</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="s">
         <v>17</v>
       </c>
-      <c r="B203" s="1">
-        <v>10</v>
-      </c>
-      <c r="C203" s="1">
+      <c r="B203" s="0">
+        <v>10</v>
+      </c>
+      <c r="C203" s="0">
         <v>95.969215393066406</v>
       </c>
     </row>
@@ -2379,10 +2377,10 @@
       <c r="A204" t="s">
         <v>17</v>
       </c>
-      <c r="B204" s="1">
-        <v>11</v>
-      </c>
-      <c r="C204" s="1">
+      <c r="B204" s="0">
+        <v>11</v>
+      </c>
+      <c r="C204" s="0">
         <v>86.566505432128906</v>
       </c>
     </row>
@@ -2390,32 +2388,32 @@
       <c r="A205" t="s">
         <v>17</v>
       </c>
-      <c r="B205" s="1">
-        <v>12</v>
-      </c>
-      <c r="C205" s="1">
-        <v>121.59109497070313</v>
+      <c r="B205" s="0">
+        <v>12</v>
+      </c>
+      <c r="C205" s="0">
+        <v>121.59109497070312</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="s">
         <v>18</v>
       </c>
-      <c r="B206" s="1">
-        <v>1</v>
-      </c>
-      <c r="C206" s="1">
-        <v>135.73043823242188</v>
+      <c r="B206" s="0">
+        <v>1</v>
+      </c>
+      <c r="C206" s="0">
+        <v>135.73043823242187</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="s">
         <v>18</v>
       </c>
-      <c r="B207" s="1">
-        <v>2</v>
-      </c>
-      <c r="C207" s="1">
+      <c r="B207" s="0">
+        <v>2</v>
+      </c>
+      <c r="C207" s="0">
         <v>119.0836181640625</v>
       </c>
     </row>
@@ -2423,10 +2421,10 @@
       <c r="A208" t="s">
         <v>18</v>
       </c>
-      <c r="B208" s="1">
-        <v>3</v>
-      </c>
-      <c r="C208" s="1">
+      <c r="B208" s="0">
+        <v>3</v>
+      </c>
+      <c r="C208" s="0">
         <v>131.49864196777344</v>
       </c>
     </row>
@@ -2434,10 +2432,10 @@
       <c r="A209" t="s">
         <v>18</v>
       </c>
-      <c r="B209" s="1">
-        <v>4</v>
-      </c>
-      <c r="C209" s="1">
+      <c r="B209" s="0">
+        <v>4</v>
+      </c>
+      <c r="C209" s="0">
         <v>170.47334289550781</v>
       </c>
     </row>
@@ -2445,10 +2443,10 @@
       <c r="A210" t="s">
         <v>18</v>
       </c>
-      <c r="B210" s="1">
-        <v>5</v>
-      </c>
-      <c r="C210" s="1">
+      <c r="B210" s="0">
+        <v>5</v>
+      </c>
+      <c r="C210" s="0">
         <v>140.91246032714844</v>
       </c>
     </row>
@@ -2456,10 +2454,10 @@
       <c r="A211" t="s">
         <v>18</v>
       </c>
-      <c r="B211" s="1">
-        <v>6</v>
-      </c>
-      <c r="C211" s="1">
+      <c r="B211" s="0">
+        <v>6</v>
+      </c>
+      <c r="C211" s="0">
         <v>148.81655883789063</v>
       </c>
     </row>
@@ -2467,10 +2465,10 @@
       <c r="A212" t="s">
         <v>18</v>
       </c>
-      <c r="B212" s="1">
-        <v>7</v>
-      </c>
-      <c r="C212" s="1">
+      <c r="B212" s="0">
+        <v>7</v>
+      </c>
+      <c r="C212" s="0">
         <v>136.10011291503906</v>
       </c>
     </row>
@@ -2478,10 +2476,10 @@
       <c r="A213" t="s">
         <v>18</v>
       </c>
-      <c r="B213" s="1">
-        <v>8</v>
-      </c>
-      <c r="C213" s="1">
+      <c r="B213" s="0">
+        <v>8</v>
+      </c>
+      <c r="C213" s="0">
         <v>86.1436767578125</v>
       </c>
     </row>
@@ -2489,10 +2487,10 @@
       <c r="A214" t="s">
         <v>18</v>
       </c>
-      <c r="B214" s="1">
-        <v>9</v>
-      </c>
-      <c r="C214" s="1">
+      <c r="B214" s="0">
+        <v>9</v>
+      </c>
+      <c r="C214" s="0">
         <v>135.07499694824219</v>
       </c>
     </row>
@@ -2500,10 +2498,10 @@
       <c r="A215" t="s">
         <v>18</v>
       </c>
-      <c r="B215" s="1">
-        <v>10</v>
-      </c>
-      <c r="C215" s="1">
+      <c r="B215" s="0">
+        <v>10</v>
+      </c>
+      <c r="C215" s="0">
         <v>89.914527893066406</v>
       </c>
     </row>
@@ -2511,10 +2509,10 @@
       <c r="A216" t="s">
         <v>18</v>
       </c>
-      <c r="B216" s="1">
-        <v>11</v>
-      </c>
-      <c r="C216" s="1">
+      <c r="B216" s="0">
+        <v>11</v>
+      </c>
+      <c r="C216" s="0">
         <v>120.86214447021484</v>
       </c>
     </row>
@@ -2522,21 +2520,21 @@
       <c r="A217" t="s">
         <v>18</v>
       </c>
-      <c r="B217" s="1">
-        <v>12</v>
-      </c>
-      <c r="C217" s="1">
-        <v>82.872787475585938</v>
+      <c r="B217" s="0">
+        <v>12</v>
+      </c>
+      <c r="C217" s="0">
+        <v>82.872787475585937</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="s">
         <v>19</v>
       </c>
-      <c r="B218" s="1">
-        <v>1</v>
-      </c>
-      <c r="C218" s="1">
+      <c r="B218" s="0">
+        <v>1</v>
+      </c>
+      <c r="C218" s="0">
         <v>135.63230895996094</v>
       </c>
     </row>
@@ -2544,10 +2542,10 @@
       <c r="A219" t="s">
         <v>19</v>
       </c>
-      <c r="B219" s="1">
-        <v>2</v>
-      </c>
-      <c r="C219" s="1">
+      <c r="B219" s="0">
+        <v>2</v>
+      </c>
+      <c r="C219" s="0">
         <v>190.81669616699219</v>
       </c>
     </row>
@@ -2555,10 +2553,10 @@
       <c r="A220" t="s">
         <v>19</v>
       </c>
-      <c r="B220" s="1">
-        <v>3</v>
-      </c>
-      <c r="C220" s="1">
+      <c r="B220" s="0">
+        <v>3</v>
+      </c>
+      <c r="C220" s="0">
         <v>290.92950439453125</v>
       </c>
     </row>
@@ -2566,10 +2564,10 @@
       <c r="A221" t="s">
         <v>19</v>
       </c>
-      <c r="B221" s="1">
-        <v>4</v>
-      </c>
-      <c r="C221" s="1">
+      <c r="B221" s="0">
+        <v>4</v>
+      </c>
+      <c r="C221" s="0">
         <v>197.17079162597656</v>
       </c>
     </row>
@@ -2577,32 +2575,32 @@
       <c r="A222" t="s">
         <v>19</v>
       </c>
-      <c r="B222" s="1">
-        <v>5</v>
-      </c>
-      <c r="C222" s="1">
-        <v>246.75491333007813</v>
+      <c r="B222" s="0">
+        <v>5</v>
+      </c>
+      <c r="C222" s="0">
+        <v>246.75491333007812</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="s">
         <v>19</v>
       </c>
-      <c r="B223" s="1">
-        <v>6</v>
-      </c>
-      <c r="C223" s="1">
-        <v>503.94247436523438</v>
+      <c r="B223" s="0">
+        <v>6</v>
+      </c>
+      <c r="C223" s="0">
+        <v>503.94247436523437</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="s">
         <v>19</v>
       </c>
-      <c r="B224" s="1">
-        <v>7</v>
-      </c>
-      <c r="C224" s="1">
+      <c r="B224" s="0">
+        <v>7</v>
+      </c>
+      <c r="C224" s="0">
         <v>558.2236328125</v>
       </c>
     </row>
@@ -2610,21 +2608,21 @@
       <c r="A225" t="s">
         <v>19</v>
       </c>
-      <c r="B225" s="1">
-        <v>8</v>
-      </c>
-      <c r="C225" s="1">
-        <v>311.36483764648438</v>
+      <c r="B225" s="0">
+        <v>8</v>
+      </c>
+      <c r="C225" s="0">
+        <v>311.36483764648437</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="s">
         <v>19</v>
       </c>
-      <c r="B226" s="1">
-        <v>9</v>
-      </c>
-      <c r="C226" s="1">
+      <c r="B226" s="0">
+        <v>9</v>
+      </c>
+      <c r="C226" s="0">
         <v>209.637939453125</v>
       </c>
     </row>
@@ -2632,10 +2630,10 @@
       <c r="A227" t="s">
         <v>19</v>
       </c>
-      <c r="B227" s="1">
-        <v>10</v>
-      </c>
-      <c r="C227" s="1">
+      <c r="B227" s="0">
+        <v>10</v>
+      </c>
+      <c r="C227" s="0">
         <v>270.02349853515625</v>
       </c>
     </row>
@@ -2643,21 +2641,21 @@
       <c r="A228" t="s">
         <v>19</v>
       </c>
-      <c r="B228" s="1">
-        <v>11</v>
-      </c>
-      <c r="C228" s="1">
-        <v>358.82839965820313</v>
+      <c r="B228" s="0">
+        <v>11</v>
+      </c>
+      <c r="C228" s="0">
+        <v>358.82839965820312</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="s">
         <v>19</v>
       </c>
-      <c r="B229" s="1">
-        <v>12</v>
-      </c>
-      <c r="C229" s="1">
+      <c r="B229" s="0">
+        <v>12</v>
+      </c>
+      <c r="C229" s="0">
         <v>196.34368896484375</v>
       </c>
     </row>
@@ -2665,10 +2663,10 @@
       <c r="A230" t="s">
         <v>20</v>
       </c>
-      <c r="B230" s="1">
-        <v>1</v>
-      </c>
-      <c r="C230" s="1">
+      <c r="B230" s="0">
+        <v>1</v>
+      </c>
+      <c r="C230" s="0">
         <v>257.848388671875</v>
       </c>
     </row>
@@ -2676,21 +2674,21 @@
       <c r="A231" t="s">
         <v>20</v>
       </c>
-      <c r="B231" s="1">
-        <v>2</v>
-      </c>
-      <c r="C231" s="1">
-        <v>194.04470825195313</v>
+      <c r="B231" s="0">
+        <v>2</v>
+      </c>
+      <c r="C231" s="0">
+        <v>194.04470825195312</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="s">
         <v>20</v>
       </c>
-      <c r="B232" s="1">
-        <v>3</v>
-      </c>
-      <c r="C232" s="1">
+      <c r="B232" s="0">
+        <v>3</v>
+      </c>
+      <c r="C232" s="0">
         <v>232.45973205566406</v>
       </c>
     </row>
@@ -2698,10 +2696,10 @@
       <c r="A233" t="s">
         <v>20</v>
       </c>
-      <c r="B233" s="1">
-        <v>4</v>
-      </c>
-      <c r="C233" s="1">
+      <c r="B233" s="0">
+        <v>4</v>
+      </c>
+      <c r="C233" s="0">
         <v>169.176025390625</v>
       </c>
     </row>
@@ -2709,10 +2707,10 @@
       <c r="A234" t="s">
         <v>20</v>
       </c>
-      <c r="B234" s="1">
-        <v>5</v>
-      </c>
-      <c r="C234" s="1">
+      <c r="B234" s="0">
+        <v>5</v>
+      </c>
+      <c r="C234" s="0">
         <v>159.40144348144531</v>
       </c>
     </row>
@@ -2720,10 +2718,10 @@
       <c r="A235" t="s">
         <v>20</v>
       </c>
-      <c r="B235" s="1">
-        <v>6</v>
-      </c>
-      <c r="C235" s="1">
+      <c r="B235" s="0">
+        <v>6</v>
+      </c>
+      <c r="C235" s="0">
         <v>318.99114990234375</v>
       </c>
     </row>
@@ -2731,10 +2729,10 @@
       <c r="A236" t="s">
         <v>20</v>
       </c>
-      <c r="B236" s="1">
-        <v>7</v>
-      </c>
-      <c r="C236" s="1">
+      <c r="B236" s="0">
+        <v>7</v>
+      </c>
+      <c r="C236" s="0">
         <v>183.65895080566406</v>
       </c>
     </row>
@@ -2742,10 +2740,10 @@
       <c r="A237" t="s">
         <v>20</v>
       </c>
-      <c r="B237" s="1">
-        <v>8</v>
-      </c>
-      <c r="C237" s="1">
+      <c r="B237" s="0">
+        <v>8</v>
+      </c>
+      <c r="C237" s="0">
         <v>151.20429992675781</v>
       </c>
     </row>
@@ -2753,10 +2751,10 @@
       <c r="A238" t="s">
         <v>20</v>
       </c>
-      <c r="B238" s="1">
-        <v>9</v>
-      </c>
-      <c r="C238" s="1">
+      <c r="B238" s="0">
+        <v>9</v>
+      </c>
+      <c r="C238" s="0">
         <v>140.77882385253906</v>
       </c>
     </row>
@@ -2764,10 +2762,10 @@
       <c r="A239" t="s">
         <v>20</v>
       </c>
-      <c r="B239" s="1">
-        <v>10</v>
-      </c>
-      <c r="C239" s="1">
+      <c r="B239" s="0">
+        <v>10</v>
+      </c>
+      <c r="C239" s="0">
         <v>184.03004455566406</v>
       </c>
     </row>
@@ -2775,10 +2773,10 @@
       <c r="A240" t="s">
         <v>20</v>
       </c>
-      <c r="B240" s="1">
-        <v>11</v>
-      </c>
-      <c r="C240" s="1">
+      <c r="B240" s="0">
+        <v>11</v>
+      </c>
+      <c r="C240" s="0">
         <v>214.97006225585938</v>
       </c>
     </row>
@@ -2786,10 +2784,10 @@
       <c r="A241" t="s">
         <v>20</v>
       </c>
-      <c r="B241" s="1">
-        <v>12</v>
-      </c>
-      <c r="C241" s="1">
+      <c r="B241" s="0">
+        <v>12</v>
+      </c>
+      <c r="C241" s="0">
         <v>160.72230529785156</v>
       </c>
     </row>
@@ -2797,10 +2795,10 @@
       <c r="A242" t="s">
         <v>21</v>
       </c>
-      <c r="B242" s="1">
-        <v>1</v>
-      </c>
-      <c r="C242" s="1">
+      <c r="B242" s="0">
+        <v>1</v>
+      </c>
+      <c r="C242" s="0">
         <v>123.15999603271484</v>
       </c>
     </row>
@@ -2808,10 +2806,10 @@
       <c r="A243" t="s">
         <v>21</v>
       </c>
-      <c r="B243" s="1">
-        <v>2</v>
-      </c>
-      <c r="C243" s="1">
+      <c r="B243" s="0">
+        <v>2</v>
+      </c>
+      <c r="C243" s="0">
         <v>109.74873352050781</v>
       </c>
     </row>
@@ -2819,10 +2817,10 @@
       <c r="A244" t="s">
         <v>21</v>
       </c>
-      <c r="B244" s="1">
-        <v>3</v>
-      </c>
-      <c r="C244" s="1">
+      <c r="B244" s="0">
+        <v>3</v>
+      </c>
+      <c r="C244" s="0">
         <v>116.60540008544922</v>
       </c>
     </row>
@@ -2830,10 +2828,10 @@
       <c r="A245" t="s">
         <v>21</v>
       </c>
-      <c r="B245" s="1">
-        <v>4</v>
-      </c>
-      <c r="C245" s="1">
+      <c r="B245" s="0">
+        <v>4</v>
+      </c>
+      <c r="C245" s="0">
         <v>102.28702545166016</v>
       </c>
     </row>
@@ -2841,10 +2839,10 @@
       <c r="A246" t="s">
         <v>21</v>
       </c>
-      <c r="B246" s="1">
-        <v>5</v>
-      </c>
-      <c r="C246" s="1">
+      <c r="B246" s="0">
+        <v>5</v>
+      </c>
+      <c r="C246" s="0">
         <v>121.543701171875</v>
       </c>
     </row>
@@ -2852,10 +2850,10 @@
       <c r="A247" t="s">
         <v>21</v>
       </c>
-      <c r="B247" s="1">
-        <v>6</v>
-      </c>
-      <c r="C247" s="1">
+      <c r="B247" s="0">
+        <v>6</v>
+      </c>
+      <c r="C247" s="0">
         <v>105.48676300048828</v>
       </c>
     </row>
@@ -2863,10 +2861,10 @@
       <c r="A248" t="s">
         <v>21</v>
       </c>
-      <c r="B248" s="1">
-        <v>7</v>
-      </c>
-      <c r="C248" s="1">
+      <c r="B248" s="0">
+        <v>7</v>
+      </c>
+      <c r="C248" s="0">
         <v>129.62263488769531</v>
       </c>
     </row>
@@ -2874,10 +2872,10 @@
       <c r="A249" t="s">
         <v>21</v>
       </c>
-      <c r="B249" s="1">
-        <v>8</v>
-      </c>
-      <c r="C249" s="1">
+      <c r="B249" s="0">
+        <v>8</v>
+      </c>
+      <c r="C249" s="0">
         <v>121.62975311279297</v>
       </c>
     </row>
@@ -2885,32 +2883,32 @@
       <c r="A250" t="s">
         <v>21</v>
       </c>
-      <c r="B250" s="1">
-        <v>9</v>
-      </c>
-      <c r="C250" s="1">
-        <v>157.31582641601563</v>
+      <c r="B250" s="0">
+        <v>9</v>
+      </c>
+      <c r="C250" s="0">
+        <v>157.31582641601562</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="s">
         <v>21</v>
       </c>
-      <c r="B251" s="1">
-        <v>10</v>
-      </c>
-      <c r="C251" s="1">
-        <v>183.25265502929688</v>
+      <c r="B251" s="0">
+        <v>10</v>
+      </c>
+      <c r="C251" s="0">
+        <v>183.25265502929687</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="s">
         <v>21</v>
       </c>
-      <c r="B252" s="1">
-        <v>11</v>
-      </c>
-      <c r="C252" s="1">
+      <c r="B252" s="0">
+        <v>11</v>
+      </c>
+      <c r="C252" s="0">
         <v>191.96647644042969</v>
       </c>
     </row>
@@ -2918,10 +2916,10 @@
       <c r="A253" t="s">
         <v>21</v>
       </c>
-      <c r="B253" s="1">
-        <v>12</v>
-      </c>
-      <c r="C253" s="1">
+      <c r="B253" s="0">
+        <v>12</v>
+      </c>
+      <c r="C253" s="0">
         <v>239.69102478027344</v>
       </c>
     </row>
@@ -2929,21 +2927,21 @@
       <c r="A254" t="s">
         <v>22</v>
       </c>
-      <c r="B254" s="1">
-        <v>1</v>
-      </c>
-      <c r="C254" s="1">
-        <v>309.97244262695313</v>
+      <c r="B254" s="0">
+        <v>1</v>
+      </c>
+      <c r="C254" s="0">
+        <v>309.97244262695312</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="s">
         <v>22</v>
       </c>
-      <c r="B255" s="1">
-        <v>2</v>
-      </c>
-      <c r="C255" s="1">
+      <c r="B255" s="0">
+        <v>2</v>
+      </c>
+      <c r="C255" s="0">
         <v>196.95947265625</v>
       </c>
     </row>
@@ -2951,10 +2949,10 @@
       <c r="A256" t="s">
         <v>22</v>
       </c>
-      <c r="B256" s="1">
-        <v>3</v>
-      </c>
-      <c r="C256" s="1">
+      <c r="B256" s="0">
+        <v>3</v>
+      </c>
+      <c r="C256" s="0">
         <v>212.78254699707031</v>
       </c>
     </row>
@@ -2962,10 +2960,10 @@
       <c r="A257" t="s">
         <v>22</v>
       </c>
-      <c r="B257" s="1">
-        <v>4</v>
-      </c>
-      <c r="C257" s="1">
+      <c r="B257" s="0">
+        <v>4</v>
+      </c>
+      <c r="C257" s="0">
         <v>135.51847839355469</v>
       </c>
     </row>
@@ -2973,10 +2971,10 @@
       <c r="A258" t="s">
         <v>22</v>
       </c>
-      <c r="B258" s="1">
-        <v>5</v>
-      </c>
-      <c r="C258" s="1">
+      <c r="B258" s="0">
+        <v>5</v>
+      </c>
+      <c r="C258" s="0">
         <v>158.68260192871094</v>
       </c>
     </row>
@@ -2984,10 +2982,10 @@
       <c r="A259" t="s">
         <v>22</v>
       </c>
-      <c r="B259" s="1">
-        <v>6</v>
-      </c>
-      <c r="C259" s="1">
+      <c r="B259" s="0">
+        <v>6</v>
+      </c>
+      <c r="C259" s="0">
         <v>149.80560302734375</v>
       </c>
     </row>
@@ -2995,10 +2993,10 @@
       <c r="A260" t="s">
         <v>22</v>
       </c>
-      <c r="B260" s="1">
-        <v>7</v>
-      </c>
-      <c r="C260" s="1">
+      <c r="B260" s="0">
+        <v>7</v>
+      </c>
+      <c r="C260" s="0">
         <v>202.04379272460938</v>
       </c>
     </row>
@@ -3006,10 +3004,10 @@
       <c r="A261" t="s">
         <v>22</v>
       </c>
-      <c r="B261" s="1">
-        <v>8</v>
-      </c>
-      <c r="C261" s="1">
+      <c r="B261" s="0">
+        <v>8</v>
+      </c>
+      <c r="C261" s="0">
         <v>238.91572570800781</v>
       </c>
     </row>
@@ -3017,21 +3015,21 @@
       <c r="A262" t="s">
         <v>22</v>
       </c>
-      <c r="B262" s="1">
-        <v>9</v>
-      </c>
-      <c r="C262" s="1">
-        <v>187.41012573242188</v>
+      <c r="B262" s="0">
+        <v>9</v>
+      </c>
+      <c r="C262" s="0">
+        <v>187.41012573242187</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="s">
         <v>22</v>
       </c>
-      <c r="B263" s="1">
-        <v>10</v>
-      </c>
-      <c r="C263" s="1">
+      <c r="B263" s="0">
+        <v>10</v>
+      </c>
+      <c r="C263" s="0">
         <v>233.31156921386719</v>
       </c>
     </row>
@@ -3039,10 +3037,10 @@
       <c r="A264" t="s">
         <v>22</v>
       </c>
-      <c r="B264" s="1">
-        <v>11</v>
-      </c>
-      <c r="C264" s="1">
+      <c r="B264" s="0">
+        <v>11</v>
+      </c>
+      <c r="C264" s="0">
         <v>205.59706115722656</v>
       </c>
     </row>
@@ -3050,21 +3048,21 @@
       <c r="A265" t="s">
         <v>22</v>
       </c>
-      <c r="B265" s="1">
-        <v>12</v>
-      </c>
-      <c r="C265" s="1">
-        <v>271.30404663085938</v>
+      <c r="B265" s="0">
+        <v>12</v>
+      </c>
+      <c r="C265" s="0">
+        <v>271.30404663085937</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="s">
         <v>23</v>
       </c>
-      <c r="B266" s="1">
-        <v>1</v>
-      </c>
-      <c r="C266" s="1">
+      <c r="B266" s="0">
+        <v>1</v>
+      </c>
+      <c r="C266" s="0">
         <v>198.156494140625</v>
       </c>
     </row>
@@ -3072,19 +3070,52 @@
       <c r="A267" t="s">
         <v>23</v>
       </c>
-      <c r="B267" s="1">
-        <v>2</v>
-      </c>
-      <c r="C267" s="1">
-        <v>137.52772521972656</v>
+      <c r="B267" s="0">
+        <v>2</v>
+      </c>
+      <c r="C267" s="0">
+        <v>139.62191772460937</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="s">
+        <v>23</v>
+      </c>
+      <c r="B268" s="0">
+        <v>3</v>
+      </c>
+      <c r="C268" s="0">
+        <v>281.207275390625</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="s">
+        <v>23</v>
+      </c>
+      <c r="B269" s="0">
+        <v>4</v>
+      </c>
+      <c r="C269" s="0">
+        <v>185.36369323730469</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="s">
+        <v>23</v>
+      </c>
+      <c r="B270" s="0">
+        <v>5</v>
+      </c>
+      <c r="C270" s="0">
+        <v>237.70785522460937</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="s">
         <v>24</v>
       </c>
-      <c r="B268" s="1"/>
-      <c r="C268" s="1"/>
+      <c r="B271" s="0"/>
+      <c r="C271" s="0"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>